<commit_message>
P07 Save/Load Option  3/17/2023 1:15 PM
</commit_message>
<xml_diff>
--- a/P07/Scrum_Sprint_3.xlsx
+++ b/P07/Scrum_Sprint_3.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="195">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -599,6 +599,12 @@
   </si>
   <si>
     <t xml:space="preserve">Completed Day 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save (via method) &amp; reload (via constructor) each obj. Cust.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git commit -m "P07 Trial Run GOOD 3/17/2023 2:54 AM"</t>
   </si>
   <si>
     <t xml:space="preserve">BONUS</t>
@@ -616,7 +622,7 @@
     <numFmt numFmtId="165" formatCode="mmm\ dd"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -725,6 +731,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -821,7 +832,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1010,6 +1021,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1090,7 +1105,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1242,11 +1257,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="97842032"/>
-        <c:axId val="55575285"/>
+        <c:axId val="65498744"/>
+        <c:axId val="71197299"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97842032"/>
+        <c:axId val="65498744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1314,12 +1329,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55575285"/>
+        <c:crossAx val="71197299"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55575285"/>
+        <c:axId val="71197299"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1396,7 +1411,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97842032"/>
+        <c:crossAx val="65498744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1423,7 +1438,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1551,11 +1566,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="17620014"/>
-        <c:axId val="25049768"/>
+        <c:axId val="6048830"/>
+        <c:axId val="68661646"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="17620014"/>
+        <c:axId val="6048830"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,7 +1636,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25049768"/>
+        <c:crossAx val="68661646"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1629,7 +1644,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25049768"/>
+        <c:axId val="68661646"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1705,7 +1720,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17620014"/>
+        <c:crossAx val="6048830"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1732,7 +1747,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1860,11 +1875,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="43231835"/>
-        <c:axId val="11606943"/>
+        <c:axId val="57194281"/>
+        <c:axId val="4356565"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43231835"/>
+        <c:axId val="57194281"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1930,7 +1945,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11606943"/>
+        <c:crossAx val="4356565"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1938,7 +1953,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11606943"/>
+        <c:axId val="4356565"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2014,7 +2029,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43231835"/>
+        <c:crossAx val="57194281"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2041,7 +2056,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2133,28 +2148,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2169,11 +2184,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="20292877"/>
-        <c:axId val="84673855"/>
+        <c:axId val="85749513"/>
+        <c:axId val="77711640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="20292877"/>
+        <c:axId val="85749513"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2239,7 +2254,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84673855"/>
+        <c:crossAx val="77711640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2247,7 +2262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84673855"/>
+        <c:axId val="77711640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2323,7 +2338,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20292877"/>
+        <c:crossAx val="85749513"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2350,7 +2365,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2478,11 +2493,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="7332983"/>
-        <c:axId val="79052837"/>
+        <c:axId val="4421478"/>
+        <c:axId val="22437851"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="7332983"/>
+        <c:axId val="4421478"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2548,7 +2563,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79052837"/>
+        <c:crossAx val="22437851"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2556,7 +2571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79052837"/>
+        <c:axId val="22437851"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2632,7 +2647,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7332983"/>
+        <c:crossAx val="4421478"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2659,7 +2674,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2787,11 +2802,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="75914584"/>
-        <c:axId val="37639006"/>
+        <c:axId val="65130411"/>
+        <c:axId val="83664050"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75914584"/>
+        <c:axId val="65130411"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2857,7 +2872,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37639006"/>
+        <c:crossAx val="83664050"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2865,7 +2880,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37639006"/>
+        <c:axId val="83664050"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2941,7 +2956,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75914584"/>
+        <c:crossAx val="65130411"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2968,7 +2983,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3096,11 +3111,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="99124332"/>
-        <c:axId val="54538070"/>
+        <c:axId val="18011139"/>
+        <c:axId val="96026979"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99124332"/>
+        <c:axId val="18011139"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3166,7 +3181,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54538070"/>
+        <c:crossAx val="96026979"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3174,7 +3189,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54538070"/>
+        <c:axId val="96026979"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3250,7 +3265,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99124332"/>
+        <c:crossAx val="18011139"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4355,7 +4370,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" s="29" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="29" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="s">
         <v>85</v>
       </c>
@@ -5498,8 +5513,8 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E7" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7935,7 +7950,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8027,7 +8042,7 @@
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -8040,7 +8055,7 @@
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">B7-C8</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -8056,7 +8071,7 @@
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">B8-C9</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -8072,7 +8087,7 @@
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">B9-C10</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -8088,11 +8103,11 @@
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">B10-C11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32"/>
@@ -8104,7 +8119,7 @@
       </c>
       <c r="B12" s="32" t="n">
         <f aca="false">B11-C12</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -8120,7 +8135,7 @@
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">B12-C13</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -8136,7 +8151,7 @@
       </c>
       <c r="B14" s="32" t="n">
         <f aca="false">B13-C14</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -8204,7 +8219,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>3</v>
       </c>
@@ -8212,19 +8227,31 @@
         <v>85</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="44"/>
+      <c r="D19" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>81</v>
+      </c>
       <c r="F19" s="45"/>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B20" s="42"/>
+      <c r="B20" s="42" t="s">
+        <v>85</v>
+      </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="45"/>
+      <c r="D20" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="F20" s="45" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -9328,7 +9355,7 @@
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="47"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="44"/>
       <c r="F18" s="45"/>
     </row>
@@ -9338,7 +9365,7 @@
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="44"/>
       <c r="F19" s="45"/>
     </row>
@@ -9348,7 +9375,7 @@
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="44"/>
       <c r="F20" s="45"/>
     </row>
@@ -9358,7 +9385,7 @@
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="44"/>
       <c r="F21" s="45"/>
     </row>
@@ -9368,7 +9395,7 @@
       </c>
       <c r="B22" s="42"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="47"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="44"/>
       <c r="F22" s="45"/>
     </row>
@@ -9378,7 +9405,7 @@
       </c>
       <c r="B23" s="42"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="47"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="44"/>
       <c r="F23" s="45"/>
     </row>
@@ -9388,7 +9415,7 @@
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="47"/>
+      <c r="D24" s="48"/>
       <c r="E24" s="44"/>
       <c r="F24" s="45"/>
     </row>
@@ -9398,7 +9425,7 @@
       </c>
       <c r="B25" s="42"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="47"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="44"/>
       <c r="F25" s="45"/>
     </row>
@@ -9408,7 +9435,7 @@
       </c>
       <c r="B26" s="42"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="47"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="44"/>
       <c r="F26" s="45"/>
     </row>
@@ -9418,7 +9445,7 @@
       </c>
       <c r="B27" s="42"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="47"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="44"/>
       <c r="F27" s="45"/>
     </row>
@@ -9428,7 +9455,7 @@
       </c>
       <c r="B28" s="42"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="47"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="44"/>
       <c r="F28" s="45"/>
     </row>
@@ -9438,7 +9465,7 @@
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="47"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="44"/>
       <c r="F29" s="45"/>
     </row>
@@ -9448,7 +9475,7 @@
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="47"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="44"/>
       <c r="F30" s="45"/>
     </row>
@@ -9458,7 +9485,7 @@
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="47"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="44"/>
       <c r="F31" s="45"/>
     </row>
@@ -9468,7 +9495,7 @@
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="47"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="44"/>
       <c r="F32" s="45"/>
     </row>
@@ -9478,7 +9505,7 @@
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="47"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="44"/>
       <c r="F33" s="45"/>
     </row>
@@ -9488,7 +9515,7 @@
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="47"/>
+      <c r="D34" s="48"/>
       <c r="E34" s="44"/>
       <c r="F34" s="45"/>
     </row>
@@ -9498,7 +9525,7 @@
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="47"/>
+      <c r="D35" s="48"/>
       <c r="E35" s="44"/>
       <c r="F35" s="45"/>
     </row>
@@ -9508,7 +9535,7 @@
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="47"/>
+      <c r="D36" s="48"/>
       <c r="E36" s="44"/>
       <c r="F36" s="45"/>
     </row>
@@ -9518,7 +9545,7 @@
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="47"/>
+      <c r="D37" s="48"/>
       <c r="E37" s="44"/>
       <c r="F37" s="45"/>
     </row>
@@ -9528,7 +9555,7 @@
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="44"/>
       <c r="F38" s="45"/>
     </row>
@@ -9538,7 +9565,7 @@
       </c>
       <c r="B39" s="42"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="44"/>
       <c r="F39" s="45"/>
     </row>
@@ -9548,7 +9575,7 @@
       </c>
       <c r="B40" s="42"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="44"/>
       <c r="F40" s="45"/>
     </row>
@@ -9558,7 +9585,7 @@
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="44"/>
       <c r="F41" s="45"/>
     </row>
@@ -9568,7 +9595,7 @@
       </c>
       <c r="B42" s="42"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="47"/>
+      <c r="D42" s="48"/>
       <c r="E42" s="44"/>
       <c r="F42" s="45"/>
     </row>
@@ -9578,7 +9605,7 @@
       </c>
       <c r="B43" s="42"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="47"/>
+      <c r="D43" s="48"/>
       <c r="E43" s="44"/>
       <c r="F43" s="45"/>
     </row>
@@ -9588,7 +9615,7 @@
       </c>
       <c r="B44" s="42"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="47"/>
+      <c r="D44" s="48"/>
       <c r="E44" s="44"/>
       <c r="F44" s="45"/>
     </row>
@@ -9598,7 +9625,7 @@
       </c>
       <c r="B45" s="42"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="47"/>
+      <c r="D45" s="48"/>
       <c r="E45" s="44"/>
       <c r="F45" s="45"/>
     </row>
@@ -9608,7 +9635,7 @@
       </c>
       <c r="B46" s="42"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="47"/>
+      <c r="D46" s="48"/>
       <c r="E46" s="44"/>
       <c r="F46" s="45"/>
     </row>
@@ -9618,7 +9645,7 @@
       </c>
       <c r="B47" s="42"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="47"/>
+      <c r="D47" s="48"/>
       <c r="E47" s="44"/>
       <c r="F47" s="45"/>
     </row>
@@ -9628,7 +9655,7 @@
       </c>
       <c r="B48" s="42"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="47"/>
+      <c r="D48" s="48"/>
       <c r="E48" s="44"/>
       <c r="F48" s="45"/>
     </row>
@@ -9638,7 +9665,7 @@
       </c>
       <c r="B49" s="42"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="47"/>
+      <c r="D49" s="48"/>
       <c r="E49" s="44"/>
       <c r="F49" s="45"/>
     </row>
@@ -9648,7 +9675,7 @@
       </c>
       <c r="B50" s="42"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="47"/>
+      <c r="D50" s="48"/>
       <c r="E50" s="44"/>
       <c r="F50" s="45"/>
     </row>
@@ -9658,7 +9685,7 @@
       </c>
       <c r="B51" s="42"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="47"/>
+      <c r="D51" s="48"/>
       <c r="E51" s="44"/>
       <c r="F51" s="45"/>
     </row>
@@ -9668,7 +9695,7 @@
       </c>
       <c r="B52" s="42"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="47"/>
+      <c r="D52" s="48"/>
       <c r="E52" s="44"/>
       <c r="F52" s="45"/>
     </row>
@@ -9678,7 +9705,7 @@
       </c>
       <c r="B53" s="42"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="47"/>
+      <c r="D53" s="48"/>
       <c r="E53" s="44"/>
       <c r="F53" s="45"/>
     </row>
@@ -9688,7 +9715,7 @@
       </c>
       <c r="B54" s="42"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="47"/>
+      <c r="D54" s="48"/>
       <c r="E54" s="44"/>
       <c r="F54" s="45"/>
     </row>
@@ -9698,7 +9725,7 @@
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="47"/>
+      <c r="D55" s="48"/>
       <c r="E55" s="44"/>
       <c r="F55" s="45"/>
     </row>
@@ -9708,7 +9735,7 @@
       </c>
       <c r="B56" s="42"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="47"/>
+      <c r="D56" s="48"/>
       <c r="E56" s="44"/>
       <c r="F56" s="45"/>
     </row>
@@ -9718,7 +9745,7 @@
       </c>
       <c r="B57" s="42"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="47"/>
+      <c r="D57" s="48"/>
       <c r="E57" s="44"/>
       <c r="F57" s="45"/>
     </row>
@@ -9728,7 +9755,7 @@
       </c>
       <c r="B58" s="42"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="47"/>
+      <c r="D58" s="48"/>
       <c r="E58" s="44"/>
       <c r="F58" s="45"/>
     </row>
@@ -9738,7 +9765,7 @@
       </c>
       <c r="B59" s="42"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="47"/>
+      <c r="D59" s="48"/>
       <c r="E59" s="44"/>
       <c r="F59" s="45"/>
     </row>
@@ -9748,7 +9775,7 @@
       </c>
       <c r="B60" s="42"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="47"/>
+      <c r="D60" s="48"/>
       <c r="E60" s="44"/>
       <c r="F60" s="45"/>
     </row>
@@ -9758,7 +9785,7 @@
       </c>
       <c r="B61" s="42"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="47"/>
+      <c r="D61" s="48"/>
       <c r="E61" s="44"/>
       <c r="F61" s="45"/>
     </row>
@@ -9768,7 +9795,7 @@
       </c>
       <c r="B62" s="42"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="47"/>
+      <c r="D62" s="48"/>
       <c r="E62" s="44"/>
       <c r="F62" s="45"/>
     </row>
@@ -9778,7 +9805,7 @@
       </c>
       <c r="B63" s="42"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="47"/>
+      <c r="D63" s="48"/>
       <c r="E63" s="44"/>
       <c r="F63" s="45"/>
     </row>
@@ -9788,7 +9815,7 @@
       </c>
       <c r="B64" s="42"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="47"/>
+      <c r="D64" s="48"/>
       <c r="E64" s="44"/>
       <c r="F64" s="45"/>
     </row>
@@ -9798,7 +9825,7 @@
       </c>
       <c r="B65" s="42"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="47"/>
+      <c r="D65" s="48"/>
       <c r="E65" s="44"/>
       <c r="F65" s="45"/>
     </row>
@@ -9808,7 +9835,7 @@
       </c>
       <c r="B66" s="42"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="47"/>
+      <c r="D66" s="48"/>
       <c r="E66" s="44"/>
       <c r="F66" s="45"/>
     </row>
@@ -9818,7 +9845,7 @@
       </c>
       <c r="B67" s="42"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="47"/>
+      <c r="D67" s="48"/>
       <c r="E67" s="44"/>
       <c r="F67" s="45"/>
     </row>
@@ -9828,7 +9855,7 @@
       </c>
       <c r="B68" s="42"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="47"/>
+      <c r="D68" s="48"/>
       <c r="E68" s="44"/>
       <c r="F68" s="45"/>
     </row>
@@ -9838,7 +9865,7 @@
       </c>
       <c r="B69" s="42"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="47"/>
+      <c r="D69" s="48"/>
       <c r="E69" s="44"/>
       <c r="F69" s="45"/>
     </row>
@@ -9848,7 +9875,7 @@
       </c>
       <c r="B70" s="42"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="47"/>
+      <c r="D70" s="48"/>
       <c r="E70" s="44"/>
       <c r="F70" s="45"/>
     </row>
@@ -9858,7 +9885,7 @@
       </c>
       <c r="B71" s="42"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="47"/>
+      <c r="D71" s="48"/>
       <c r="E71" s="44"/>
       <c r="F71" s="45"/>
     </row>
@@ -9868,7 +9895,7 @@
       </c>
       <c r="B72" s="42"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="47"/>
+      <c r="D72" s="48"/>
       <c r="E72" s="44"/>
       <c r="F72" s="45"/>
     </row>
@@ -9878,7 +9905,7 @@
       </c>
       <c r="B73" s="42"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="47"/>
+      <c r="D73" s="48"/>
       <c r="E73" s="44"/>
       <c r="F73" s="45"/>
     </row>
@@ -9888,7 +9915,7 @@
       </c>
       <c r="B74" s="42"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="47"/>
+      <c r="D74" s="48"/>
       <c r="E74" s="44"/>
       <c r="F74" s="45"/>
     </row>
@@ -9898,7 +9925,7 @@
       </c>
       <c r="B75" s="42"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="47"/>
+      <c r="D75" s="48"/>
       <c r="E75" s="44"/>
       <c r="F75" s="45"/>
     </row>
@@ -9908,7 +9935,7 @@
       </c>
       <c r="B76" s="42"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="47"/>
+      <c r="D76" s="48"/>
       <c r="E76" s="44"/>
       <c r="F76" s="45"/>
     </row>
@@ -9918,7 +9945,7 @@
       </c>
       <c r="B77" s="42"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="47"/>
+      <c r="D77" s="48"/>
       <c r="E77" s="44"/>
       <c r="F77" s="45"/>
     </row>
@@ -9928,7 +9955,7 @@
       </c>
       <c r="B78" s="42"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="47"/>
+      <c r="D78" s="48"/>
       <c r="E78" s="44"/>
       <c r="F78" s="45"/>
     </row>
@@ -9938,7 +9965,7 @@
       </c>
       <c r="B79" s="42"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="47"/>
+      <c r="D79" s="48"/>
       <c r="E79" s="44"/>
       <c r="F79" s="45"/>
     </row>
@@ -9948,7 +9975,7 @@
       </c>
       <c r="B80" s="42"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="47"/>
+      <c r="D80" s="48"/>
       <c r="E80" s="44"/>
       <c r="F80" s="45"/>
     </row>
@@ -9958,7 +9985,7 @@
       </c>
       <c r="B81" s="42"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="47"/>
+      <c r="D81" s="48"/>
       <c r="E81" s="44"/>
       <c r="F81" s="45"/>
     </row>
@@ -9968,7 +9995,7 @@
       </c>
       <c r="B82" s="42"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="47"/>
+      <c r="D82" s="48"/>
       <c r="E82" s="44"/>
       <c r="F82" s="45"/>
     </row>
@@ -9978,7 +10005,7 @@
       </c>
       <c r="B83" s="42"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="47"/>
+      <c r="D83" s="48"/>
       <c r="E83" s="44"/>
       <c r="F83" s="45"/>
     </row>
@@ -9988,7 +10015,7 @@
       </c>
       <c r="B84" s="42"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="47"/>
+      <c r="D84" s="48"/>
       <c r="E84" s="44"/>
       <c r="F84" s="45"/>
     </row>
@@ -9998,7 +10025,7 @@
       </c>
       <c r="B85" s="42"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="47"/>
+      <c r="D85" s="48"/>
       <c r="E85" s="44"/>
       <c r="F85" s="45"/>
     </row>
@@ -10008,7 +10035,7 @@
       </c>
       <c r="B86" s="42"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="47"/>
+      <c r="D86" s="48"/>
       <c r="E86" s="44"/>
       <c r="F86" s="45"/>
     </row>
@@ -10018,7 +10045,7 @@
       </c>
       <c r="B87" s="42"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="47"/>
+      <c r="D87" s="48"/>
       <c r="E87" s="44"/>
       <c r="F87" s="45"/>
     </row>
@@ -10028,7 +10055,7 @@
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="47"/>
+      <c r="D88" s="48"/>
       <c r="E88" s="44"/>
       <c r="F88" s="45"/>
     </row>
@@ -10038,7 +10065,7 @@
       </c>
       <c r="B89" s="42"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="47"/>
+      <c r="D89" s="48"/>
       <c r="E89" s="44"/>
       <c r="F89" s="45"/>
     </row>
@@ -10048,7 +10075,7 @@
       </c>
       <c r="B90" s="42"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="47"/>
+      <c r="D90" s="48"/>
       <c r="E90" s="44"/>
       <c r="F90" s="45"/>
     </row>
@@ -10058,7 +10085,7 @@
       </c>
       <c r="B91" s="42"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="47"/>
+      <c r="D91" s="48"/>
       <c r="E91" s="44"/>
       <c r="F91" s="45"/>
     </row>
@@ -10068,7 +10095,7 @@
       </c>
       <c r="B92" s="42"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="47"/>
+      <c r="D92" s="48"/>
       <c r="E92" s="44"/>
       <c r="F92" s="45"/>
     </row>
@@ -10078,7 +10105,7 @@
       </c>
       <c r="B93" s="42"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="47"/>
+      <c r="D93" s="48"/>
       <c r="E93" s="44"/>
       <c r="F93" s="45"/>
     </row>
@@ -10088,7 +10115,7 @@
       </c>
       <c r="B94" s="42"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="47"/>
+      <c r="D94" s="48"/>
       <c r="E94" s="44"/>
       <c r="F94" s="45"/>
     </row>
@@ -10098,7 +10125,7 @@
       </c>
       <c r="B95" s="42"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="47"/>
+      <c r="D95" s="48"/>
       <c r="E95" s="44"/>
       <c r="F95" s="45"/>
     </row>
@@ -10108,7 +10135,7 @@
       </c>
       <c r="B96" s="42"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="47"/>
+      <c r="D96" s="48"/>
       <c r="E96" s="44"/>
       <c r="F96" s="45"/>
     </row>
@@ -10118,7 +10145,7 @@
       </c>
       <c r="B97" s="42"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="47"/>
+      <c r="D97" s="48"/>
       <c r="E97" s="44"/>
       <c r="F97" s="45"/>
     </row>
@@ -10128,7 +10155,7 @@
       </c>
       <c r="B98" s="42"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="47"/>
+      <c r="D98" s="48"/>
       <c r="E98" s="44"/>
       <c r="F98" s="45"/>
     </row>
@@ -10138,7 +10165,7 @@
       </c>
       <c r="B99" s="42"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="47"/>
+      <c r="D99" s="48"/>
       <c r="E99" s="44"/>
       <c r="F99" s="45"/>
     </row>
@@ -10148,7 +10175,7 @@
       </c>
       <c r="B100" s="42"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="47"/>
+      <c r="D100" s="48"/>
       <c r="E100" s="44"/>
       <c r="F100" s="45"/>
     </row>
@@ -10455,7 +10482,7 @@
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="47"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="44"/>
       <c r="F18" s="45"/>
     </row>
@@ -10465,7 +10492,7 @@
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="44"/>
       <c r="F19" s="45"/>
     </row>
@@ -10475,7 +10502,7 @@
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="44"/>
       <c r="F20" s="45"/>
     </row>
@@ -10485,7 +10512,7 @@
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="44"/>
       <c r="F21" s="45"/>
     </row>
@@ -10495,7 +10522,7 @@
       </c>
       <c r="B22" s="42"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="47"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="44"/>
       <c r="F22" s="45"/>
     </row>
@@ -10505,7 +10532,7 @@
       </c>
       <c r="B23" s="42"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="47"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="44"/>
       <c r="F23" s="45"/>
     </row>
@@ -10515,7 +10542,7 @@
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="47"/>
+      <c r="D24" s="48"/>
       <c r="E24" s="44"/>
       <c r="F24" s="45"/>
     </row>
@@ -10525,7 +10552,7 @@
       </c>
       <c r="B25" s="42"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="47"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="44"/>
       <c r="F25" s="45"/>
     </row>
@@ -10535,7 +10562,7 @@
       </c>
       <c r="B26" s="42"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="47"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="44"/>
       <c r="F26" s="45"/>
     </row>
@@ -10545,7 +10572,7 @@
       </c>
       <c r="B27" s="42"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="47"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="44"/>
       <c r="F27" s="45"/>
     </row>
@@ -10555,7 +10582,7 @@
       </c>
       <c r="B28" s="42"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="47"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="44"/>
       <c r="F28" s="45"/>
     </row>
@@ -10565,7 +10592,7 @@
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="47"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="44"/>
       <c r="F29" s="45"/>
     </row>
@@ -10575,7 +10602,7 @@
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="47"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="44"/>
       <c r="F30" s="45"/>
     </row>
@@ -10585,7 +10612,7 @@
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="47"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="44"/>
       <c r="F31" s="45"/>
     </row>
@@ -10595,7 +10622,7 @@
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="47"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="44"/>
       <c r="F32" s="45"/>
     </row>
@@ -10605,7 +10632,7 @@
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="47"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="44"/>
       <c r="F33" s="45"/>
     </row>
@@ -10615,7 +10642,7 @@
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="47"/>
+      <c r="D34" s="48"/>
       <c r="E34" s="44"/>
       <c r="F34" s="45"/>
     </row>
@@ -10625,7 +10652,7 @@
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="47"/>
+      <c r="D35" s="48"/>
       <c r="E35" s="44"/>
       <c r="F35" s="45"/>
     </row>
@@ -10635,7 +10662,7 @@
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="47"/>
+      <c r="D36" s="48"/>
       <c r="E36" s="44"/>
       <c r="F36" s="45"/>
     </row>
@@ -10645,7 +10672,7 @@
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="47"/>
+      <c r="D37" s="48"/>
       <c r="E37" s="44"/>
       <c r="F37" s="45"/>
     </row>
@@ -10655,7 +10682,7 @@
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="44"/>
       <c r="F38" s="45"/>
     </row>
@@ -10665,7 +10692,7 @@
       </c>
       <c r="B39" s="42"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="44"/>
       <c r="F39" s="45"/>
     </row>
@@ -10675,7 +10702,7 @@
       </c>
       <c r="B40" s="42"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="44"/>
       <c r="F40" s="45"/>
     </row>
@@ -10685,7 +10712,7 @@
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="44"/>
       <c r="F41" s="45"/>
     </row>
@@ -10695,7 +10722,7 @@
       </c>
       <c r="B42" s="42"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="47"/>
+      <c r="D42" s="48"/>
       <c r="E42" s="44"/>
       <c r="F42" s="45"/>
     </row>
@@ -10705,7 +10732,7 @@
       </c>
       <c r="B43" s="42"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="47"/>
+      <c r="D43" s="48"/>
       <c r="E43" s="44"/>
       <c r="F43" s="45"/>
     </row>
@@ -10715,7 +10742,7 @@
       </c>
       <c r="B44" s="42"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="47"/>
+      <c r="D44" s="48"/>
       <c r="E44" s="44"/>
       <c r="F44" s="45"/>
     </row>
@@ -10725,7 +10752,7 @@
       </c>
       <c r="B45" s="42"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="47"/>
+      <c r="D45" s="48"/>
       <c r="E45" s="44"/>
       <c r="F45" s="45"/>
     </row>
@@ -10735,7 +10762,7 @@
       </c>
       <c r="B46" s="42"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="47"/>
+      <c r="D46" s="48"/>
       <c r="E46" s="44"/>
       <c r="F46" s="45"/>
     </row>
@@ -10745,7 +10772,7 @@
       </c>
       <c r="B47" s="42"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="47"/>
+      <c r="D47" s="48"/>
       <c r="E47" s="44"/>
       <c r="F47" s="45"/>
     </row>
@@ -10755,7 +10782,7 @@
       </c>
       <c r="B48" s="42"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="47"/>
+      <c r="D48" s="48"/>
       <c r="E48" s="44"/>
       <c r="F48" s="45"/>
     </row>
@@ -10765,7 +10792,7 @@
       </c>
       <c r="B49" s="42"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="47"/>
+      <c r="D49" s="48"/>
       <c r="E49" s="44"/>
       <c r="F49" s="45"/>
     </row>
@@ -10775,7 +10802,7 @@
       </c>
       <c r="B50" s="42"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="47"/>
+      <c r="D50" s="48"/>
       <c r="E50" s="44"/>
       <c r="F50" s="45"/>
     </row>
@@ -10785,7 +10812,7 @@
       </c>
       <c r="B51" s="42"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="47"/>
+      <c r="D51" s="48"/>
       <c r="E51" s="44"/>
       <c r="F51" s="45"/>
     </row>
@@ -10795,7 +10822,7 @@
       </c>
       <c r="B52" s="42"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="47"/>
+      <c r="D52" s="48"/>
       <c r="E52" s="44"/>
       <c r="F52" s="45"/>
     </row>
@@ -10805,7 +10832,7 @@
       </c>
       <c r="B53" s="42"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="47"/>
+      <c r="D53" s="48"/>
       <c r="E53" s="44"/>
       <c r="F53" s="45"/>
     </row>
@@ -10815,7 +10842,7 @@
       </c>
       <c r="B54" s="42"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="47"/>
+      <c r="D54" s="48"/>
       <c r="E54" s="44"/>
       <c r="F54" s="45"/>
     </row>
@@ -10825,7 +10852,7 @@
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="47"/>
+      <c r="D55" s="48"/>
       <c r="E55" s="44"/>
       <c r="F55" s="45"/>
     </row>
@@ -10835,7 +10862,7 @@
       </c>
       <c r="B56" s="42"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="47"/>
+      <c r="D56" s="48"/>
       <c r="E56" s="44"/>
       <c r="F56" s="45"/>
     </row>
@@ -10845,7 +10872,7 @@
       </c>
       <c r="B57" s="42"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="47"/>
+      <c r="D57" s="48"/>
       <c r="E57" s="44"/>
       <c r="F57" s="45"/>
     </row>
@@ -10855,7 +10882,7 @@
       </c>
       <c r="B58" s="42"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="47"/>
+      <c r="D58" s="48"/>
       <c r="E58" s="44"/>
       <c r="F58" s="45"/>
     </row>
@@ -10865,7 +10892,7 @@
       </c>
       <c r="B59" s="42"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="47"/>
+      <c r="D59" s="48"/>
       <c r="E59" s="44"/>
       <c r="F59" s="45"/>
     </row>
@@ -10875,7 +10902,7 @@
       </c>
       <c r="B60" s="42"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="47"/>
+      <c r="D60" s="48"/>
       <c r="E60" s="44"/>
       <c r="F60" s="45"/>
     </row>
@@ -10885,7 +10912,7 @@
       </c>
       <c r="B61" s="42"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="47"/>
+      <c r="D61" s="48"/>
       <c r="E61" s="44"/>
       <c r="F61" s="45"/>
     </row>
@@ -10895,7 +10922,7 @@
       </c>
       <c r="B62" s="42"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="47"/>
+      <c r="D62" s="48"/>
       <c r="E62" s="44"/>
       <c r="F62" s="45"/>
     </row>
@@ -10905,7 +10932,7 @@
       </c>
       <c r="B63" s="42"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="47"/>
+      <c r="D63" s="48"/>
       <c r="E63" s="44"/>
       <c r="F63" s="45"/>
     </row>
@@ -10915,7 +10942,7 @@
       </c>
       <c r="B64" s="42"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="47"/>
+      <c r="D64" s="48"/>
       <c r="E64" s="44"/>
       <c r="F64" s="45"/>
     </row>
@@ -10925,7 +10952,7 @@
       </c>
       <c r="B65" s="42"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="47"/>
+      <c r="D65" s="48"/>
       <c r="E65" s="44"/>
       <c r="F65" s="45"/>
     </row>
@@ -10935,7 +10962,7 @@
       </c>
       <c r="B66" s="42"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="47"/>
+      <c r="D66" s="48"/>
       <c r="E66" s="44"/>
       <c r="F66" s="45"/>
     </row>
@@ -10945,7 +10972,7 @@
       </c>
       <c r="B67" s="42"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="47"/>
+      <c r="D67" s="48"/>
       <c r="E67" s="44"/>
       <c r="F67" s="45"/>
     </row>
@@ -10955,7 +10982,7 @@
       </c>
       <c r="B68" s="42"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="47"/>
+      <c r="D68" s="48"/>
       <c r="E68" s="44"/>
       <c r="F68" s="45"/>
     </row>
@@ -10965,7 +10992,7 @@
       </c>
       <c r="B69" s="42"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="47"/>
+      <c r="D69" s="48"/>
       <c r="E69" s="44"/>
       <c r="F69" s="45"/>
     </row>
@@ -10975,7 +11002,7 @@
       </c>
       <c r="B70" s="42"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="47"/>
+      <c r="D70" s="48"/>
       <c r="E70" s="44"/>
       <c r="F70" s="45"/>
     </row>
@@ -10985,7 +11012,7 @@
       </c>
       <c r="B71" s="42"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="47"/>
+      <c r="D71" s="48"/>
       <c r="E71" s="44"/>
       <c r="F71" s="45"/>
     </row>
@@ -10995,7 +11022,7 @@
       </c>
       <c r="B72" s="42"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="47"/>
+      <c r="D72" s="48"/>
       <c r="E72" s="44"/>
       <c r="F72" s="45"/>
     </row>
@@ -11005,7 +11032,7 @@
       </c>
       <c r="B73" s="42"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="47"/>
+      <c r="D73" s="48"/>
       <c r="E73" s="44"/>
       <c r="F73" s="45"/>
     </row>
@@ -11015,7 +11042,7 @@
       </c>
       <c r="B74" s="42"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="47"/>
+      <c r="D74" s="48"/>
       <c r="E74" s="44"/>
       <c r="F74" s="45"/>
     </row>
@@ -11025,7 +11052,7 @@
       </c>
       <c r="B75" s="42"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="47"/>
+      <c r="D75" s="48"/>
       <c r="E75" s="44"/>
       <c r="F75" s="45"/>
     </row>
@@ -11035,7 +11062,7 @@
       </c>
       <c r="B76" s="42"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="47"/>
+      <c r="D76" s="48"/>
       <c r="E76" s="44"/>
       <c r="F76" s="45"/>
     </row>
@@ -11045,7 +11072,7 @@
       </c>
       <c r="B77" s="42"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="47"/>
+      <c r="D77" s="48"/>
       <c r="E77" s="44"/>
       <c r="F77" s="45"/>
     </row>
@@ -11055,7 +11082,7 @@
       </c>
       <c r="B78" s="42"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="47"/>
+      <c r="D78" s="48"/>
       <c r="E78" s="44"/>
       <c r="F78" s="45"/>
     </row>
@@ -11065,7 +11092,7 @@
       </c>
       <c r="B79" s="42"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="47"/>
+      <c r="D79" s="48"/>
       <c r="E79" s="44"/>
       <c r="F79" s="45"/>
     </row>
@@ -11075,7 +11102,7 @@
       </c>
       <c r="B80" s="42"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="47"/>
+      <c r="D80" s="48"/>
       <c r="E80" s="44"/>
       <c r="F80" s="45"/>
     </row>
@@ -11085,7 +11112,7 @@
       </c>
       <c r="B81" s="42"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="47"/>
+      <c r="D81" s="48"/>
       <c r="E81" s="44"/>
       <c r="F81" s="45"/>
     </row>
@@ -11095,7 +11122,7 @@
       </c>
       <c r="B82" s="42"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="47"/>
+      <c r="D82" s="48"/>
       <c r="E82" s="44"/>
       <c r="F82" s="45"/>
     </row>
@@ -11105,7 +11132,7 @@
       </c>
       <c r="B83" s="42"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="47"/>
+      <c r="D83" s="48"/>
       <c r="E83" s="44"/>
       <c r="F83" s="45"/>
     </row>
@@ -11115,7 +11142,7 @@
       </c>
       <c r="B84" s="42"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="47"/>
+      <c r="D84" s="48"/>
       <c r="E84" s="44"/>
       <c r="F84" s="45"/>
     </row>
@@ -11125,7 +11152,7 @@
       </c>
       <c r="B85" s="42"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="47"/>
+      <c r="D85" s="48"/>
       <c r="E85" s="44"/>
       <c r="F85" s="45"/>
     </row>
@@ -11135,7 +11162,7 @@
       </c>
       <c r="B86" s="42"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="47"/>
+      <c r="D86" s="48"/>
       <c r="E86" s="44"/>
       <c r="F86" s="45"/>
     </row>
@@ -11145,7 +11172,7 @@
       </c>
       <c r="B87" s="42"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="47"/>
+      <c r="D87" s="48"/>
       <c r="E87" s="44"/>
       <c r="F87" s="45"/>
     </row>
@@ -11155,7 +11182,7 @@
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="47"/>
+      <c r="D88" s="48"/>
       <c r="E88" s="44"/>
       <c r="F88" s="45"/>
     </row>
@@ -11165,7 +11192,7 @@
       </c>
       <c r="B89" s="42"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="47"/>
+      <c r="D89" s="48"/>
       <c r="E89" s="44"/>
       <c r="F89" s="45"/>
     </row>
@@ -11175,7 +11202,7 @@
       </c>
       <c r="B90" s="42"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="47"/>
+      <c r="D90" s="48"/>
       <c r="E90" s="44"/>
       <c r="F90" s="45"/>
     </row>
@@ -11185,7 +11212,7 @@
       </c>
       <c r="B91" s="42"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="47"/>
+      <c r="D91" s="48"/>
       <c r="E91" s="44"/>
       <c r="F91" s="45"/>
     </row>
@@ -11195,7 +11222,7 @@
       </c>
       <c r="B92" s="42"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="47"/>
+      <c r="D92" s="48"/>
       <c r="E92" s="44"/>
       <c r="F92" s="45"/>
     </row>
@@ -11205,7 +11232,7 @@
       </c>
       <c r="B93" s="42"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="47"/>
+      <c r="D93" s="48"/>
       <c r="E93" s="44"/>
       <c r="F93" s="45"/>
     </row>
@@ -11215,7 +11242,7 @@
       </c>
       <c r="B94" s="42"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="47"/>
+      <c r="D94" s="48"/>
       <c r="E94" s="44"/>
       <c r="F94" s="45"/>
     </row>
@@ -11225,7 +11252,7 @@
       </c>
       <c r="B95" s="42"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="47"/>
+      <c r="D95" s="48"/>
       <c r="E95" s="44"/>
       <c r="F95" s="45"/>
     </row>
@@ -11235,7 +11262,7 @@
       </c>
       <c r="B96" s="42"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="47"/>
+      <c r="D96" s="48"/>
       <c r="E96" s="44"/>
       <c r="F96" s="45"/>
     </row>
@@ -11245,7 +11272,7 @@
       </c>
       <c r="B97" s="42"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="47"/>
+      <c r="D97" s="48"/>
       <c r="E97" s="44"/>
       <c r="F97" s="45"/>
     </row>
@@ -11255,7 +11282,7 @@
       </c>
       <c r="B98" s="42"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="47"/>
+      <c r="D98" s="48"/>
       <c r="E98" s="44"/>
       <c r="F98" s="45"/>
     </row>
@@ -11265,7 +11292,7 @@
       </c>
       <c r="B99" s="42"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="47"/>
+      <c r="D99" s="48"/>
       <c r="E99" s="44"/>
       <c r="F99" s="45"/>
     </row>
@@ -11275,7 +11302,7 @@
       </c>
       <c r="B100" s="42"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="47"/>
+      <c r="D100" s="48"/>
       <c r="E100" s="44"/>
       <c r="F100" s="45"/>
     </row>
@@ -11345,8 +11372,8 @@
         <f aca="false">'Sprint 05 Backlog'!B1+1</f>
         <v>6</v>
       </c>
-      <c r="C1" s="48" t="s">
-        <v>191</v>
+      <c r="C1" s="49" t="s">
+        <v>193</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>2</v>
@@ -11542,8 +11569,8 @@
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
-      <c r="D15" s="48" t="s">
-        <v>192</v>
+      <c r="D15" s="49" t="s">
+        <v>194</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>
@@ -11586,7 +11613,7 @@
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="47"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="44"/>
       <c r="F18" s="45"/>
     </row>
@@ -11596,7 +11623,7 @@
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="44"/>
       <c r="F19" s="45"/>
     </row>
@@ -11606,7 +11633,7 @@
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="44"/>
       <c r="F20" s="45"/>
     </row>
@@ -11616,7 +11643,7 @@
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="44"/>
       <c r="F21" s="45"/>
     </row>
@@ -11626,7 +11653,7 @@
       </c>
       <c r="B22" s="42"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="47"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="44"/>
       <c r="F22" s="45"/>
     </row>
@@ -11636,7 +11663,7 @@
       </c>
       <c r="B23" s="42"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="47"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="44"/>
       <c r="F23" s="45"/>
     </row>
@@ -11646,7 +11673,7 @@
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="47"/>
+      <c r="D24" s="48"/>
       <c r="E24" s="44"/>
       <c r="F24" s="45"/>
     </row>
@@ -11656,7 +11683,7 @@
       </c>
       <c r="B25" s="42"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="47"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="44"/>
       <c r="F25" s="45"/>
     </row>
@@ -11666,7 +11693,7 @@
       </c>
       <c r="B26" s="42"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="47"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="44"/>
       <c r="F26" s="45"/>
     </row>
@@ -11676,7 +11703,7 @@
       </c>
       <c r="B27" s="42"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="47"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="44"/>
       <c r="F27" s="45"/>
     </row>
@@ -11686,7 +11713,7 @@
       </c>
       <c r="B28" s="42"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="47"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="44"/>
       <c r="F28" s="45"/>
     </row>
@@ -11696,7 +11723,7 @@
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="47"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="44"/>
       <c r="F29" s="45"/>
     </row>
@@ -11706,7 +11733,7 @@
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="47"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="44"/>
       <c r="F30" s="45"/>
     </row>
@@ -11716,7 +11743,7 @@
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="47"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="44"/>
       <c r="F31" s="45"/>
     </row>
@@ -11726,7 +11753,7 @@
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="47"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="44"/>
       <c r="F32" s="45"/>
     </row>
@@ -11736,7 +11763,7 @@
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="47"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="44"/>
       <c r="F33" s="45"/>
     </row>
@@ -11746,7 +11773,7 @@
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="47"/>
+      <c r="D34" s="48"/>
       <c r="E34" s="44"/>
       <c r="F34" s="45"/>
     </row>
@@ -11756,7 +11783,7 @@
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="47"/>
+      <c r="D35" s="48"/>
       <c r="E35" s="44"/>
       <c r="F35" s="45"/>
     </row>
@@ -11766,7 +11793,7 @@
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="47"/>
+      <c r="D36" s="48"/>
       <c r="E36" s="44"/>
       <c r="F36" s="45"/>
     </row>
@@ -11776,7 +11803,7 @@
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="47"/>
+      <c r="D37" s="48"/>
       <c r="E37" s="44"/>
       <c r="F37" s="45"/>
     </row>
@@ -11786,7 +11813,7 @@
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="44"/>
       <c r="F38" s="45"/>
     </row>
@@ -11796,7 +11823,7 @@
       </c>
       <c r="B39" s="42"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="44"/>
       <c r="F39" s="45"/>
     </row>
@@ -11806,7 +11833,7 @@
       </c>
       <c r="B40" s="42"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="44"/>
       <c r="F40" s="45"/>
     </row>
@@ -11816,7 +11843,7 @@
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="44"/>
       <c r="F41" s="45"/>
     </row>
@@ -11826,7 +11853,7 @@
       </c>
       <c r="B42" s="42"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="47"/>
+      <c r="D42" s="48"/>
       <c r="E42" s="44"/>
       <c r="F42" s="45"/>
     </row>
@@ -11836,7 +11863,7 @@
       </c>
       <c r="B43" s="42"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="47"/>
+      <c r="D43" s="48"/>
       <c r="E43" s="44"/>
       <c r="F43" s="45"/>
     </row>
@@ -11846,7 +11873,7 @@
       </c>
       <c r="B44" s="42"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="47"/>
+      <c r="D44" s="48"/>
       <c r="E44" s="44"/>
       <c r="F44" s="45"/>
     </row>
@@ -11856,7 +11883,7 @@
       </c>
       <c r="B45" s="42"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="47"/>
+      <c r="D45" s="48"/>
       <c r="E45" s="44"/>
       <c r="F45" s="45"/>
     </row>
@@ -11866,7 +11893,7 @@
       </c>
       <c r="B46" s="42"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="47"/>
+      <c r="D46" s="48"/>
       <c r="E46" s="44"/>
       <c r="F46" s="45"/>
     </row>
@@ -11876,7 +11903,7 @@
       </c>
       <c r="B47" s="42"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="47"/>
+      <c r="D47" s="48"/>
       <c r="E47" s="44"/>
       <c r="F47" s="45"/>
     </row>
@@ -11886,7 +11913,7 @@
       </c>
       <c r="B48" s="42"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="47"/>
+      <c r="D48" s="48"/>
       <c r="E48" s="44"/>
       <c r="F48" s="45"/>
     </row>
@@ -11896,7 +11923,7 @@
       </c>
       <c r="B49" s="42"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="47"/>
+      <c r="D49" s="48"/>
       <c r="E49" s="44"/>
       <c r="F49" s="45"/>
     </row>
@@ -11906,7 +11933,7 @@
       </c>
       <c r="B50" s="42"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="47"/>
+      <c r="D50" s="48"/>
       <c r="E50" s="44"/>
       <c r="F50" s="45"/>
     </row>
@@ -11916,7 +11943,7 @@
       </c>
       <c r="B51" s="42"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="47"/>
+      <c r="D51" s="48"/>
       <c r="E51" s="44"/>
       <c r="F51" s="45"/>
     </row>
@@ -11926,7 +11953,7 @@
       </c>
       <c r="B52" s="42"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="47"/>
+      <c r="D52" s="48"/>
       <c r="E52" s="44"/>
       <c r="F52" s="45"/>
     </row>
@@ -11936,7 +11963,7 @@
       </c>
       <c r="B53" s="42"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="47"/>
+      <c r="D53" s="48"/>
       <c r="E53" s="44"/>
       <c r="F53" s="45"/>
     </row>
@@ -11946,7 +11973,7 @@
       </c>
       <c r="B54" s="42"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="47"/>
+      <c r="D54" s="48"/>
       <c r="E54" s="44"/>
       <c r="F54" s="45"/>
     </row>
@@ -11956,7 +11983,7 @@
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="47"/>
+      <c r="D55" s="48"/>
       <c r="E55" s="44"/>
       <c r="F55" s="45"/>
     </row>
@@ -11966,7 +11993,7 @@
       </c>
       <c r="B56" s="42"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="47"/>
+      <c r="D56" s="48"/>
       <c r="E56" s="44"/>
       <c r="F56" s="45"/>
     </row>
@@ -11976,7 +12003,7 @@
       </c>
       <c r="B57" s="42"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="47"/>
+      <c r="D57" s="48"/>
       <c r="E57" s="44"/>
       <c r="F57" s="45"/>
     </row>
@@ -11986,7 +12013,7 @@
       </c>
       <c r="B58" s="42"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="47"/>
+      <c r="D58" s="48"/>
       <c r="E58" s="44"/>
       <c r="F58" s="45"/>
     </row>
@@ -11996,7 +12023,7 @@
       </c>
       <c r="B59" s="42"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="47"/>
+      <c r="D59" s="48"/>
       <c r="E59" s="44"/>
       <c r="F59" s="45"/>
     </row>
@@ -12006,7 +12033,7 @@
       </c>
       <c r="B60" s="42"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="47"/>
+      <c r="D60" s="48"/>
       <c r="E60" s="44"/>
       <c r="F60" s="45"/>
     </row>
@@ -12016,7 +12043,7 @@
       </c>
       <c r="B61" s="42"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="47"/>
+      <c r="D61" s="48"/>
       <c r="E61" s="44"/>
       <c r="F61" s="45"/>
     </row>
@@ -12026,7 +12053,7 @@
       </c>
       <c r="B62" s="42"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="47"/>
+      <c r="D62" s="48"/>
       <c r="E62" s="44"/>
       <c r="F62" s="45"/>
     </row>
@@ -12036,7 +12063,7 @@
       </c>
       <c r="B63" s="42"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="47"/>
+      <c r="D63" s="48"/>
       <c r="E63" s="44"/>
       <c r="F63" s="45"/>
     </row>
@@ -12046,7 +12073,7 @@
       </c>
       <c r="B64" s="42"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="47"/>
+      <c r="D64" s="48"/>
       <c r="E64" s="44"/>
       <c r="F64" s="45"/>
     </row>
@@ -12056,7 +12083,7 @@
       </c>
       <c r="B65" s="42"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="47"/>
+      <c r="D65" s="48"/>
       <c r="E65" s="44"/>
       <c r="F65" s="45"/>
     </row>
@@ -12066,7 +12093,7 @@
       </c>
       <c r="B66" s="42"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="47"/>
+      <c r="D66" s="48"/>
       <c r="E66" s="44"/>
       <c r="F66" s="45"/>
     </row>
@@ -12076,7 +12103,7 @@
       </c>
       <c r="B67" s="42"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="47"/>
+      <c r="D67" s="48"/>
       <c r="E67" s="44"/>
       <c r="F67" s="45"/>
     </row>
@@ -12086,7 +12113,7 @@
       </c>
       <c r="B68" s="42"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="47"/>
+      <c r="D68" s="48"/>
       <c r="E68" s="44"/>
       <c r="F68" s="45"/>
     </row>
@@ -12096,7 +12123,7 @@
       </c>
       <c r="B69" s="42"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="47"/>
+      <c r="D69" s="48"/>
       <c r="E69" s="44"/>
       <c r="F69" s="45"/>
     </row>
@@ -12106,7 +12133,7 @@
       </c>
       <c r="B70" s="42"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="47"/>
+      <c r="D70" s="48"/>
       <c r="E70" s="44"/>
       <c r="F70" s="45"/>
     </row>
@@ -12116,7 +12143,7 @@
       </c>
       <c r="B71" s="42"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="47"/>
+      <c r="D71" s="48"/>
       <c r="E71" s="44"/>
       <c r="F71" s="45"/>
     </row>
@@ -12126,7 +12153,7 @@
       </c>
       <c r="B72" s="42"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="47"/>
+      <c r="D72" s="48"/>
       <c r="E72" s="44"/>
       <c r="F72" s="45"/>
     </row>
@@ -12136,7 +12163,7 @@
       </c>
       <c r="B73" s="42"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="47"/>
+      <c r="D73" s="48"/>
       <c r="E73" s="44"/>
       <c r="F73" s="45"/>
     </row>
@@ -12146,7 +12173,7 @@
       </c>
       <c r="B74" s="42"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="47"/>
+      <c r="D74" s="48"/>
       <c r="E74" s="44"/>
       <c r="F74" s="45"/>
     </row>
@@ -12156,7 +12183,7 @@
       </c>
       <c r="B75" s="42"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="47"/>
+      <c r="D75" s="48"/>
       <c r="E75" s="44"/>
       <c r="F75" s="45"/>
     </row>
@@ -12166,7 +12193,7 @@
       </c>
       <c r="B76" s="42"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="47"/>
+      <c r="D76" s="48"/>
       <c r="E76" s="44"/>
       <c r="F76" s="45"/>
     </row>
@@ -12176,7 +12203,7 @@
       </c>
       <c r="B77" s="42"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="47"/>
+      <c r="D77" s="48"/>
       <c r="E77" s="44"/>
       <c r="F77" s="45"/>
     </row>
@@ -12186,7 +12213,7 @@
       </c>
       <c r="B78" s="42"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="47"/>
+      <c r="D78" s="48"/>
       <c r="E78" s="44"/>
       <c r="F78" s="45"/>
     </row>
@@ -12196,7 +12223,7 @@
       </c>
       <c r="B79" s="42"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="47"/>
+      <c r="D79" s="48"/>
       <c r="E79" s="44"/>
       <c r="F79" s="45"/>
     </row>
@@ -12206,7 +12233,7 @@
       </c>
       <c r="B80" s="42"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="47"/>
+      <c r="D80" s="48"/>
       <c r="E80" s="44"/>
       <c r="F80" s="45"/>
     </row>
@@ -12216,7 +12243,7 @@
       </c>
       <c r="B81" s="42"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="47"/>
+      <c r="D81" s="48"/>
       <c r="E81" s="44"/>
       <c r="F81" s="45"/>
     </row>
@@ -12226,7 +12253,7 @@
       </c>
       <c r="B82" s="42"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="47"/>
+      <c r="D82" s="48"/>
       <c r="E82" s="44"/>
       <c r="F82" s="45"/>
     </row>
@@ -12236,7 +12263,7 @@
       </c>
       <c r="B83" s="42"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="47"/>
+      <c r="D83" s="48"/>
       <c r="E83" s="44"/>
       <c r="F83" s="45"/>
     </row>
@@ -12246,7 +12273,7 @@
       </c>
       <c r="B84" s="42"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="47"/>
+      <c r="D84" s="48"/>
       <c r="E84" s="44"/>
       <c r="F84" s="45"/>
     </row>
@@ -12256,7 +12283,7 @@
       </c>
       <c r="B85" s="42"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="47"/>
+      <c r="D85" s="48"/>
       <c r="E85" s="44"/>
       <c r="F85" s="45"/>
     </row>
@@ -12266,7 +12293,7 @@
       </c>
       <c r="B86" s="42"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="47"/>
+      <c r="D86" s="48"/>
       <c r="E86" s="44"/>
       <c r="F86" s="45"/>
     </row>
@@ -12276,7 +12303,7 @@
       </c>
       <c r="B87" s="42"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="47"/>
+      <c r="D87" s="48"/>
       <c r="E87" s="44"/>
       <c r="F87" s="45"/>
     </row>
@@ -12286,7 +12313,7 @@
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="47"/>
+      <c r="D88" s="48"/>
       <c r="E88" s="44"/>
       <c r="F88" s="45"/>
     </row>
@@ -12296,7 +12323,7 @@
       </c>
       <c r="B89" s="42"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="47"/>
+      <c r="D89" s="48"/>
       <c r="E89" s="44"/>
       <c r="F89" s="45"/>
     </row>
@@ -12306,7 +12333,7 @@
       </c>
       <c r="B90" s="42"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="47"/>
+      <c r="D90" s="48"/>
       <c r="E90" s="44"/>
       <c r="F90" s="45"/>
     </row>
@@ -12316,7 +12343,7 @@
       </c>
       <c r="B91" s="42"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="47"/>
+      <c r="D91" s="48"/>
       <c r="E91" s="44"/>
       <c r="F91" s="45"/>
     </row>
@@ -12326,7 +12353,7 @@
       </c>
       <c r="B92" s="42"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="47"/>
+      <c r="D92" s="48"/>
       <c r="E92" s="44"/>
       <c r="F92" s="45"/>
     </row>
@@ -12336,7 +12363,7 @@
       </c>
       <c r="B93" s="42"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="47"/>
+      <c r="D93" s="48"/>
       <c r="E93" s="44"/>
       <c r="F93" s="45"/>
     </row>
@@ -12346,7 +12373,7 @@
       </c>
       <c r="B94" s="42"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="47"/>
+      <c r="D94" s="48"/>
       <c r="E94" s="44"/>
       <c r="F94" s="45"/>
     </row>
@@ -12356,7 +12383,7 @@
       </c>
       <c r="B95" s="42"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="47"/>
+      <c r="D95" s="48"/>
       <c r="E95" s="44"/>
       <c r="F95" s="45"/>
     </row>
@@ -12366,7 +12393,7 @@
       </c>
       <c r="B96" s="42"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="47"/>
+      <c r="D96" s="48"/>
       <c r="E96" s="44"/>
       <c r="F96" s="45"/>
     </row>
@@ -12376,7 +12403,7 @@
       </c>
       <c r="B97" s="42"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="47"/>
+      <c r="D97" s="48"/>
       <c r="E97" s="44"/>
       <c r="F97" s="45"/>
     </row>
@@ -12386,7 +12413,7 @@
       </c>
       <c r="B98" s="42"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="47"/>
+      <c r="D98" s="48"/>
       <c r="E98" s="44"/>
       <c r="F98" s="45"/>
     </row>
@@ -12396,7 +12423,7 @@
       </c>
       <c r="B99" s="42"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="47"/>
+      <c r="D99" s="48"/>
       <c r="E99" s="44"/>
       <c r="F99" s="45"/>
     </row>
@@ -12406,7 +12433,7 @@
       </c>
       <c r="B100" s="42"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="47"/>
+      <c r="D100" s="48"/>
       <c r="E100" s="44"/>
       <c r="F100" s="45"/>
     </row>

</xml_diff>

<commit_message>
P07 Save/Load Order  3/18/2023 1:15 AM
</commit_message>
<xml_diff>
--- a/P07/Scrum_Sprint_3.xlsx
+++ b/P07/Scrum_Sprint_3.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="197">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -605,6 +605,12 @@
   </si>
   <si>
     <t xml:space="preserve">git commit -m "P07 Trial Run GOOD 3/17/2023 2:54 AM"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save (via method) &amp; reload (via constructor) each obj. Opt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git commit -m "P07 Save/Load Option 3/17/2023 1:15 PM"</t>
   </si>
   <si>
     <t xml:space="preserve">BONUS</t>
@@ -622,7 +628,7 @@
     <numFmt numFmtId="165" formatCode="mmm\ dd"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -731,11 +737,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -832,7 +833,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1021,10 +1022,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1151,10 +1148,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0822345810160595"/>
-          <c:y val="0.16191074795726"/>
-          <c:w val="0.884146722489533"/>
-          <c:h val="0.635449402891263"/>
+          <c:x val="0.082244859696269"/>
+          <c:y val="0.161931103847121"/>
+          <c:w val="0.884069745640897"/>
+          <c:h val="0.635403570530551"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1257,11 +1254,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="65498744"/>
-        <c:axId val="71197299"/>
+        <c:axId val="99758733"/>
+        <c:axId val="90488292"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65498744"/>
+        <c:axId val="99758733"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1329,12 +1326,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71197299"/>
+        <c:crossAx val="90488292"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71197299"/>
+        <c:axId val="90488292"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1411,7 +1408,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65498744"/>
+        <c:crossAx val="99758733"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1566,11 +1563,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="6048830"/>
-        <c:axId val="68661646"/>
+        <c:axId val="29661122"/>
+        <c:axId val="53172241"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6048830"/>
+        <c:axId val="29661122"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,7 +1633,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68661646"/>
+        <c:crossAx val="53172241"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1644,7 +1641,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68661646"/>
+        <c:axId val="53172241"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1720,7 +1717,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6048830"/>
+        <c:crossAx val="29661122"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1875,11 +1872,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="57194281"/>
-        <c:axId val="4356565"/>
+        <c:axId val="68411361"/>
+        <c:axId val="21569018"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57194281"/>
+        <c:axId val="68411361"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1945,7 +1942,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4356565"/>
+        <c:crossAx val="21569018"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1953,7 +1950,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4356565"/>
+        <c:axId val="21569018"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2029,7 +2026,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57194281"/>
+        <c:crossAx val="68411361"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2148,28 +2145,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2184,11 +2181,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="85749513"/>
-        <c:axId val="77711640"/>
+        <c:axId val="13889259"/>
+        <c:axId val="76327102"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85749513"/>
+        <c:axId val="13889259"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2254,7 +2251,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77711640"/>
+        <c:crossAx val="76327102"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2262,7 +2259,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77711640"/>
+        <c:axId val="76327102"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2338,7 +2335,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85749513"/>
+        <c:crossAx val="13889259"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2493,11 +2490,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="4421478"/>
-        <c:axId val="22437851"/>
+        <c:axId val="28573326"/>
+        <c:axId val="81280412"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4421478"/>
+        <c:axId val="28573326"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2563,7 +2560,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22437851"/>
+        <c:crossAx val="81280412"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2571,7 +2568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22437851"/>
+        <c:axId val="81280412"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2647,7 +2644,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4421478"/>
+        <c:crossAx val="28573326"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2802,11 +2799,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="65130411"/>
-        <c:axId val="83664050"/>
+        <c:axId val="32991939"/>
+        <c:axId val="58960274"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="65130411"/>
+        <c:axId val="32991939"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2872,7 +2869,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83664050"/>
+        <c:crossAx val="58960274"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2880,7 +2877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83664050"/>
+        <c:axId val="58960274"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2956,7 +2953,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65130411"/>
+        <c:crossAx val="32991939"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3111,11 +3108,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="18011139"/>
-        <c:axId val="96026979"/>
+        <c:axId val="72057821"/>
+        <c:axId val="68008980"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="18011139"/>
+        <c:axId val="72057821"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3181,7 +3178,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96026979"/>
+        <c:crossAx val="68008980"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3189,7 +3186,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96026979"/>
+        <c:axId val="68008980"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3265,7 +3262,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18011139"/>
+        <c:crossAx val="72057821"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3303,9 +3300,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1904400</xdr:colOff>
+      <xdr:colOff>1904040</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>119160</xdr:rowOff>
+      <xdr:rowOff>118800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3313,8 +3310,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9125280" y="275040"/>
-        <a:ext cx="5760720" cy="2863440"/>
+        <a:off x="9123120" y="275040"/>
+        <a:ext cx="5760000" cy="2863080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3338,9 +3335,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1771920</xdr:colOff>
+      <xdr:colOff>1771560</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3348,8 +3345,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="457920"/>
-        <a:ext cx="3750840" cy="1846800"/>
+        <a:off x="4090680" y="457920"/>
+        <a:ext cx="3751200" cy="1846440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3373,9 +3370,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517320</xdr:colOff>
+      <xdr:colOff>516960</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3383,8 +3380,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="457920"/>
-        <a:ext cx="3746160" cy="1846800"/>
+        <a:off x="4090680" y="457920"/>
+        <a:ext cx="3746520" cy="1846440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3408,9 +3405,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517320</xdr:colOff>
+      <xdr:colOff>516960</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3418,8 +3415,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="458280"/>
-        <a:ext cx="3746160" cy="1846800"/>
+        <a:off x="4090680" y="458280"/>
+        <a:ext cx="3746520" cy="1846440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3443,9 +3440,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517320</xdr:colOff>
+      <xdr:colOff>516960</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3453,8 +3450,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="457920"/>
-        <a:ext cx="3746160" cy="1846800"/>
+        <a:off x="4090680" y="457920"/>
+        <a:ext cx="3746520" cy="1846440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3478,9 +3475,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517320</xdr:colOff>
+      <xdr:colOff>516960</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3488,8 +3485,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="457920"/>
-        <a:ext cx="3746160" cy="1846800"/>
+        <a:off x="4090680" y="457920"/>
+        <a:ext cx="3746520" cy="1846440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3513,9 +3510,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517320</xdr:colOff>
+      <xdr:colOff>516960</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3523,8 +3520,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="457920"/>
-        <a:ext cx="3746160" cy="1846800"/>
+        <a:off x="4090680" y="457920"/>
+        <a:ext cx="3746520" cy="1846440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3556,12 +3553,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="62.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="62.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="1" width="11.57"/>
   </cols>
   <sheetData>
@@ -5517,7 +5514,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -6790,7 +6787,7 @@
       <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -7949,11 +7946,11 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8042,7 +8039,7 @@
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -8055,7 +8052,7 @@
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">B7-C8</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C8" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -8071,7 +8068,7 @@
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">B8-C9</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C9" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -8087,7 +8084,7 @@
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">B9-C10</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C10" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -8103,11 +8100,11 @@
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">B10-C11</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32"/>
@@ -8119,7 +8116,7 @@
       </c>
       <c r="B12" s="32" t="n">
         <f aca="false">B11-C12</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -8135,7 +8132,7 @@
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">B12-C13</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -8151,7 +8148,7 @@
       </c>
       <c r="B14" s="32" t="n">
         <f aca="false">B13-C14</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -8227,7 +8224,7 @@
         <v>85</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="47" t="s">
+      <c r="D19" s="46" t="s">
         <v>191</v>
       </c>
       <c r="E19" s="44" t="s">
@@ -8253,34 +8250,54 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="42"/>
+      <c r="B21" s="42" t="s">
+        <v>85</v>
+      </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="44"/>
+      <c r="D21" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>159</v>
+      </c>
       <c r="F21" s="45"/>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B22" s="42"/>
+      <c r="B22" s="42" t="s">
+        <v>85</v>
+      </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="45"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B23" s="42"/>
+      <c r="B23" s="42" t="s">
+        <v>85</v>
+      </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="44"/>
+      <c r="D23" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>159</v>
+      </c>
       <c r="F23" s="45"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9102,7 +9119,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9355,7 +9372,7 @@
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="48"/>
+      <c r="D18" s="47"/>
       <c r="E18" s="44"/>
       <c r="F18" s="45"/>
     </row>
@@ -9365,7 +9382,7 @@
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="48"/>
+      <c r="D19" s="47"/>
       <c r="E19" s="44"/>
       <c r="F19" s="45"/>
     </row>
@@ -9375,7 +9392,7 @@
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="48"/>
+      <c r="D20" s="47"/>
       <c r="E20" s="44"/>
       <c r="F20" s="45"/>
     </row>
@@ -9385,7 +9402,7 @@
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="48"/>
+      <c r="D21" s="47"/>
       <c r="E21" s="44"/>
       <c r="F21" s="45"/>
     </row>
@@ -9395,7 +9412,7 @@
       </c>
       <c r="B22" s="42"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="48"/>
+      <c r="D22" s="47"/>
       <c r="E22" s="44"/>
       <c r="F22" s="45"/>
     </row>
@@ -9405,7 +9422,7 @@
       </c>
       <c r="B23" s="42"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="48"/>
+      <c r="D23" s="47"/>
       <c r="E23" s="44"/>
       <c r="F23" s="45"/>
     </row>
@@ -9415,7 +9432,7 @@
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="48"/>
+      <c r="D24" s="47"/>
       <c r="E24" s="44"/>
       <c r="F24" s="45"/>
     </row>
@@ -9425,7 +9442,7 @@
       </c>
       <c r="B25" s="42"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="48"/>
+      <c r="D25" s="47"/>
       <c r="E25" s="44"/>
       <c r="F25" s="45"/>
     </row>
@@ -9435,7 +9452,7 @@
       </c>
       <c r="B26" s="42"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="48"/>
+      <c r="D26" s="47"/>
       <c r="E26" s="44"/>
       <c r="F26" s="45"/>
     </row>
@@ -9445,7 +9462,7 @@
       </c>
       <c r="B27" s="42"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="48"/>
+      <c r="D27" s="47"/>
       <c r="E27" s="44"/>
       <c r="F27" s="45"/>
     </row>
@@ -9455,7 +9472,7 @@
       </c>
       <c r="B28" s="42"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="48"/>
+      <c r="D28" s="47"/>
       <c r="E28" s="44"/>
       <c r="F28" s="45"/>
     </row>
@@ -9465,7 +9482,7 @@
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="48"/>
+      <c r="D29" s="47"/>
       <c r="E29" s="44"/>
       <c r="F29" s="45"/>
     </row>
@@ -9475,7 +9492,7 @@
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="48"/>
+      <c r="D30" s="47"/>
       <c r="E30" s="44"/>
       <c r="F30" s="45"/>
     </row>
@@ -9485,7 +9502,7 @@
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="48"/>
+      <c r="D31" s="47"/>
       <c r="E31" s="44"/>
       <c r="F31" s="45"/>
     </row>
@@ -9495,7 +9512,7 @@
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="48"/>
+      <c r="D32" s="47"/>
       <c r="E32" s="44"/>
       <c r="F32" s="45"/>
     </row>
@@ -9505,7 +9522,7 @@
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="48"/>
+      <c r="D33" s="47"/>
       <c r="E33" s="44"/>
       <c r="F33" s="45"/>
     </row>
@@ -9515,7 +9532,7 @@
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="48"/>
+      <c r="D34" s="47"/>
       <c r="E34" s="44"/>
       <c r="F34" s="45"/>
     </row>
@@ -9525,7 +9542,7 @@
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="48"/>
+      <c r="D35" s="47"/>
       <c r="E35" s="44"/>
       <c r="F35" s="45"/>
     </row>
@@ -9535,7 +9552,7 @@
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="48"/>
+      <c r="D36" s="47"/>
       <c r="E36" s="44"/>
       <c r="F36" s="45"/>
     </row>
@@ -9545,7 +9562,7 @@
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="48"/>
+      <c r="D37" s="47"/>
       <c r="E37" s="44"/>
       <c r="F37" s="45"/>
     </row>
@@ -9555,7 +9572,7 @@
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="48"/>
+      <c r="D38" s="47"/>
       <c r="E38" s="44"/>
       <c r="F38" s="45"/>
     </row>
@@ -9565,7 +9582,7 @@
       </c>
       <c r="B39" s="42"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="48"/>
+      <c r="D39" s="47"/>
       <c r="E39" s="44"/>
       <c r="F39" s="45"/>
     </row>
@@ -9575,7 +9592,7 @@
       </c>
       <c r="B40" s="42"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="48"/>
+      <c r="D40" s="47"/>
       <c r="E40" s="44"/>
       <c r="F40" s="45"/>
     </row>
@@ -9585,7 +9602,7 @@
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="48"/>
+      <c r="D41" s="47"/>
       <c r="E41" s="44"/>
       <c r="F41" s="45"/>
     </row>
@@ -9595,7 +9612,7 @@
       </c>
       <c r="B42" s="42"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="48"/>
+      <c r="D42" s="47"/>
       <c r="E42" s="44"/>
       <c r="F42" s="45"/>
     </row>
@@ -9605,7 +9622,7 @@
       </c>
       <c r="B43" s="42"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="48"/>
+      <c r="D43" s="47"/>
       <c r="E43" s="44"/>
       <c r="F43" s="45"/>
     </row>
@@ -9615,7 +9632,7 @@
       </c>
       <c r="B44" s="42"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="48"/>
+      <c r="D44" s="47"/>
       <c r="E44" s="44"/>
       <c r="F44" s="45"/>
     </row>
@@ -9625,7 +9642,7 @@
       </c>
       <c r="B45" s="42"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="48"/>
+      <c r="D45" s="47"/>
       <c r="E45" s="44"/>
       <c r="F45" s="45"/>
     </row>
@@ -9635,7 +9652,7 @@
       </c>
       <c r="B46" s="42"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="48"/>
+      <c r="D46" s="47"/>
       <c r="E46" s="44"/>
       <c r="F46" s="45"/>
     </row>
@@ -9645,7 +9662,7 @@
       </c>
       <c r="B47" s="42"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="48"/>
+      <c r="D47" s="47"/>
       <c r="E47" s="44"/>
       <c r="F47" s="45"/>
     </row>
@@ -9655,7 +9672,7 @@
       </c>
       <c r="B48" s="42"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="48"/>
+      <c r="D48" s="47"/>
       <c r="E48" s="44"/>
       <c r="F48" s="45"/>
     </row>
@@ -9665,7 +9682,7 @@
       </c>
       <c r="B49" s="42"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="48"/>
+      <c r="D49" s="47"/>
       <c r="E49" s="44"/>
       <c r="F49" s="45"/>
     </row>
@@ -9675,7 +9692,7 @@
       </c>
       <c r="B50" s="42"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="48"/>
+      <c r="D50" s="47"/>
       <c r="E50" s="44"/>
       <c r="F50" s="45"/>
     </row>
@@ -9685,7 +9702,7 @@
       </c>
       <c r="B51" s="42"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="48"/>
+      <c r="D51" s="47"/>
       <c r="E51" s="44"/>
       <c r="F51" s="45"/>
     </row>
@@ -9695,7 +9712,7 @@
       </c>
       <c r="B52" s="42"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="48"/>
+      <c r="D52" s="47"/>
       <c r="E52" s="44"/>
       <c r="F52" s="45"/>
     </row>
@@ -9705,7 +9722,7 @@
       </c>
       <c r="B53" s="42"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="48"/>
+      <c r="D53" s="47"/>
       <c r="E53" s="44"/>
       <c r="F53" s="45"/>
     </row>
@@ -9715,7 +9732,7 @@
       </c>
       <c r="B54" s="42"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="48"/>
+      <c r="D54" s="47"/>
       <c r="E54" s="44"/>
       <c r="F54" s="45"/>
     </row>
@@ -9725,7 +9742,7 @@
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="48"/>
+      <c r="D55" s="47"/>
       <c r="E55" s="44"/>
       <c r="F55" s="45"/>
     </row>
@@ -9735,7 +9752,7 @@
       </c>
       <c r="B56" s="42"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="48"/>
+      <c r="D56" s="47"/>
       <c r="E56" s="44"/>
       <c r="F56" s="45"/>
     </row>
@@ -9745,7 +9762,7 @@
       </c>
       <c r="B57" s="42"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="48"/>
+      <c r="D57" s="47"/>
       <c r="E57" s="44"/>
       <c r="F57" s="45"/>
     </row>
@@ -9755,7 +9772,7 @@
       </c>
       <c r="B58" s="42"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="48"/>
+      <c r="D58" s="47"/>
       <c r="E58" s="44"/>
       <c r="F58" s="45"/>
     </row>
@@ -9765,7 +9782,7 @@
       </c>
       <c r="B59" s="42"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="48"/>
+      <c r="D59" s="47"/>
       <c r="E59" s="44"/>
       <c r="F59" s="45"/>
     </row>
@@ -9775,7 +9792,7 @@
       </c>
       <c r="B60" s="42"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="48"/>
+      <c r="D60" s="47"/>
       <c r="E60" s="44"/>
       <c r="F60" s="45"/>
     </row>
@@ -9785,7 +9802,7 @@
       </c>
       <c r="B61" s="42"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="48"/>
+      <c r="D61" s="47"/>
       <c r="E61" s="44"/>
       <c r="F61" s="45"/>
     </row>
@@ -9795,7 +9812,7 @@
       </c>
       <c r="B62" s="42"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="48"/>
+      <c r="D62" s="47"/>
       <c r="E62" s="44"/>
       <c r="F62" s="45"/>
     </row>
@@ -9805,7 +9822,7 @@
       </c>
       <c r="B63" s="42"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="48"/>
+      <c r="D63" s="47"/>
       <c r="E63" s="44"/>
       <c r="F63" s="45"/>
     </row>
@@ -9815,7 +9832,7 @@
       </c>
       <c r="B64" s="42"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="48"/>
+      <c r="D64" s="47"/>
       <c r="E64" s="44"/>
       <c r="F64" s="45"/>
     </row>
@@ -9825,7 +9842,7 @@
       </c>
       <c r="B65" s="42"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="48"/>
+      <c r="D65" s="47"/>
       <c r="E65" s="44"/>
       <c r="F65" s="45"/>
     </row>
@@ -9835,7 +9852,7 @@
       </c>
       <c r="B66" s="42"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="48"/>
+      <c r="D66" s="47"/>
       <c r="E66" s="44"/>
       <c r="F66" s="45"/>
     </row>
@@ -9845,7 +9862,7 @@
       </c>
       <c r="B67" s="42"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="48"/>
+      <c r="D67" s="47"/>
       <c r="E67" s="44"/>
       <c r="F67" s="45"/>
     </row>
@@ -9855,7 +9872,7 @@
       </c>
       <c r="B68" s="42"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="48"/>
+      <c r="D68" s="47"/>
       <c r="E68" s="44"/>
       <c r="F68" s="45"/>
     </row>
@@ -9865,7 +9882,7 @@
       </c>
       <c r="B69" s="42"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="48"/>
+      <c r="D69" s="47"/>
       <c r="E69" s="44"/>
       <c r="F69" s="45"/>
     </row>
@@ -9875,7 +9892,7 @@
       </c>
       <c r="B70" s="42"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="48"/>
+      <c r="D70" s="47"/>
       <c r="E70" s="44"/>
       <c r="F70" s="45"/>
     </row>
@@ -9885,7 +9902,7 @@
       </c>
       <c r="B71" s="42"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="48"/>
+      <c r="D71" s="47"/>
       <c r="E71" s="44"/>
       <c r="F71" s="45"/>
     </row>
@@ -9895,7 +9912,7 @@
       </c>
       <c r="B72" s="42"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="48"/>
+      <c r="D72" s="47"/>
       <c r="E72" s="44"/>
       <c r="F72" s="45"/>
     </row>
@@ -9905,7 +9922,7 @@
       </c>
       <c r="B73" s="42"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="48"/>
+      <c r="D73" s="47"/>
       <c r="E73" s="44"/>
       <c r="F73" s="45"/>
     </row>
@@ -9915,7 +9932,7 @@
       </c>
       <c r="B74" s="42"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="48"/>
+      <c r="D74" s="47"/>
       <c r="E74" s="44"/>
       <c r="F74" s="45"/>
     </row>
@@ -9925,7 +9942,7 @@
       </c>
       <c r="B75" s="42"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="48"/>
+      <c r="D75" s="47"/>
       <c r="E75" s="44"/>
       <c r="F75" s="45"/>
     </row>
@@ -9935,7 +9952,7 @@
       </c>
       <c r="B76" s="42"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="48"/>
+      <c r="D76" s="47"/>
       <c r="E76" s="44"/>
       <c r="F76" s="45"/>
     </row>
@@ -9945,7 +9962,7 @@
       </c>
       <c r="B77" s="42"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="48"/>
+      <c r="D77" s="47"/>
       <c r="E77" s="44"/>
       <c r="F77" s="45"/>
     </row>
@@ -9955,7 +9972,7 @@
       </c>
       <c r="B78" s="42"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="48"/>
+      <c r="D78" s="47"/>
       <c r="E78" s="44"/>
       <c r="F78" s="45"/>
     </row>
@@ -9965,7 +9982,7 @@
       </c>
       <c r="B79" s="42"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="48"/>
+      <c r="D79" s="47"/>
       <c r="E79" s="44"/>
       <c r="F79" s="45"/>
     </row>
@@ -9975,7 +9992,7 @@
       </c>
       <c r="B80" s="42"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="48"/>
+      <c r="D80" s="47"/>
       <c r="E80" s="44"/>
       <c r="F80" s="45"/>
     </row>
@@ -9985,7 +10002,7 @@
       </c>
       <c r="B81" s="42"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="48"/>
+      <c r="D81" s="47"/>
       <c r="E81" s="44"/>
       <c r="F81" s="45"/>
     </row>
@@ -9995,7 +10012,7 @@
       </c>
       <c r="B82" s="42"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="48"/>
+      <c r="D82" s="47"/>
       <c r="E82" s="44"/>
       <c r="F82" s="45"/>
     </row>
@@ -10005,7 +10022,7 @@
       </c>
       <c r="B83" s="42"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="48"/>
+      <c r="D83" s="47"/>
       <c r="E83" s="44"/>
       <c r="F83" s="45"/>
     </row>
@@ -10015,7 +10032,7 @@
       </c>
       <c r="B84" s="42"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="48"/>
+      <c r="D84" s="47"/>
       <c r="E84" s="44"/>
       <c r="F84" s="45"/>
     </row>
@@ -10025,7 +10042,7 @@
       </c>
       <c r="B85" s="42"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="48"/>
+      <c r="D85" s="47"/>
       <c r="E85" s="44"/>
       <c r="F85" s="45"/>
     </row>
@@ -10035,7 +10052,7 @@
       </c>
       <c r="B86" s="42"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="48"/>
+      <c r="D86" s="47"/>
       <c r="E86" s="44"/>
       <c r="F86" s="45"/>
     </row>
@@ -10045,7 +10062,7 @@
       </c>
       <c r="B87" s="42"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="48"/>
+      <c r="D87" s="47"/>
       <c r="E87" s="44"/>
       <c r="F87" s="45"/>
     </row>
@@ -10055,7 +10072,7 @@
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="48"/>
+      <c r="D88" s="47"/>
       <c r="E88" s="44"/>
       <c r="F88" s="45"/>
     </row>
@@ -10065,7 +10082,7 @@
       </c>
       <c r="B89" s="42"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="48"/>
+      <c r="D89" s="47"/>
       <c r="E89" s="44"/>
       <c r="F89" s="45"/>
     </row>
@@ -10075,7 +10092,7 @@
       </c>
       <c r="B90" s="42"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="48"/>
+      <c r="D90" s="47"/>
       <c r="E90" s="44"/>
       <c r="F90" s="45"/>
     </row>
@@ -10085,7 +10102,7 @@
       </c>
       <c r="B91" s="42"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="48"/>
+      <c r="D91" s="47"/>
       <c r="E91" s="44"/>
       <c r="F91" s="45"/>
     </row>
@@ -10095,7 +10112,7 @@
       </c>
       <c r="B92" s="42"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="48"/>
+      <c r="D92" s="47"/>
       <c r="E92" s="44"/>
       <c r="F92" s="45"/>
     </row>
@@ -10105,7 +10122,7 @@
       </c>
       <c r="B93" s="42"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="48"/>
+      <c r="D93" s="47"/>
       <c r="E93" s="44"/>
       <c r="F93" s="45"/>
     </row>
@@ -10115,7 +10132,7 @@
       </c>
       <c r="B94" s="42"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="48"/>
+      <c r="D94" s="47"/>
       <c r="E94" s="44"/>
       <c r="F94" s="45"/>
     </row>
@@ -10125,7 +10142,7 @@
       </c>
       <c r="B95" s="42"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="48"/>
+      <c r="D95" s="47"/>
       <c r="E95" s="44"/>
       <c r="F95" s="45"/>
     </row>
@@ -10135,7 +10152,7 @@
       </c>
       <c r="B96" s="42"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="48"/>
+      <c r="D96" s="47"/>
       <c r="E96" s="44"/>
       <c r="F96" s="45"/>
     </row>
@@ -10145,7 +10162,7 @@
       </c>
       <c r="B97" s="42"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="48"/>
+      <c r="D97" s="47"/>
       <c r="E97" s="44"/>
       <c r="F97" s="45"/>
     </row>
@@ -10155,7 +10172,7 @@
       </c>
       <c r="B98" s="42"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="48"/>
+      <c r="D98" s="47"/>
       <c r="E98" s="44"/>
       <c r="F98" s="45"/>
     </row>
@@ -10165,7 +10182,7 @@
       </c>
       <c r="B99" s="42"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="48"/>
+      <c r="D99" s="47"/>
       <c r="E99" s="44"/>
       <c r="F99" s="45"/>
     </row>
@@ -10175,7 +10192,7 @@
       </c>
       <c r="B100" s="42"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="48"/>
+      <c r="D100" s="47"/>
       <c r="E100" s="44"/>
       <c r="F100" s="45"/>
     </row>
@@ -10228,7 +10245,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -10482,7 +10499,7 @@
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="48"/>
+      <c r="D18" s="47"/>
       <c r="E18" s="44"/>
       <c r="F18" s="45"/>
     </row>
@@ -10492,7 +10509,7 @@
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="48"/>
+      <c r="D19" s="47"/>
       <c r="E19" s="44"/>
       <c r="F19" s="45"/>
     </row>
@@ -10502,7 +10519,7 @@
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="48"/>
+      <c r="D20" s="47"/>
       <c r="E20" s="44"/>
       <c r="F20" s="45"/>
     </row>
@@ -10512,7 +10529,7 @@
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="48"/>
+      <c r="D21" s="47"/>
       <c r="E21" s="44"/>
       <c r="F21" s="45"/>
     </row>
@@ -10522,7 +10539,7 @@
       </c>
       <c r="B22" s="42"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="48"/>
+      <c r="D22" s="47"/>
       <c r="E22" s="44"/>
       <c r="F22" s="45"/>
     </row>
@@ -10532,7 +10549,7 @@
       </c>
       <c r="B23" s="42"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="48"/>
+      <c r="D23" s="47"/>
       <c r="E23" s="44"/>
       <c r="F23" s="45"/>
     </row>
@@ -10542,7 +10559,7 @@
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="48"/>
+      <c r="D24" s="47"/>
       <c r="E24" s="44"/>
       <c r="F24" s="45"/>
     </row>
@@ -10552,7 +10569,7 @@
       </c>
       <c r="B25" s="42"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="48"/>
+      <c r="D25" s="47"/>
       <c r="E25" s="44"/>
       <c r="F25" s="45"/>
     </row>
@@ -10562,7 +10579,7 @@
       </c>
       <c r="B26" s="42"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="48"/>
+      <c r="D26" s="47"/>
       <c r="E26" s="44"/>
       <c r="F26" s="45"/>
     </row>
@@ -10572,7 +10589,7 @@
       </c>
       <c r="B27" s="42"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="48"/>
+      <c r="D27" s="47"/>
       <c r="E27" s="44"/>
       <c r="F27" s="45"/>
     </row>
@@ -10582,7 +10599,7 @@
       </c>
       <c r="B28" s="42"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="48"/>
+      <c r="D28" s="47"/>
       <c r="E28" s="44"/>
       <c r="F28" s="45"/>
     </row>
@@ -10592,7 +10609,7 @@
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="48"/>
+      <c r="D29" s="47"/>
       <c r="E29" s="44"/>
       <c r="F29" s="45"/>
     </row>
@@ -10602,7 +10619,7 @@
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="48"/>
+      <c r="D30" s="47"/>
       <c r="E30" s="44"/>
       <c r="F30" s="45"/>
     </row>
@@ -10612,7 +10629,7 @@
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="48"/>
+      <c r="D31" s="47"/>
       <c r="E31" s="44"/>
       <c r="F31" s="45"/>
     </row>
@@ -10622,7 +10639,7 @@
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="48"/>
+      <c r="D32" s="47"/>
       <c r="E32" s="44"/>
       <c r="F32" s="45"/>
     </row>
@@ -10632,7 +10649,7 @@
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="48"/>
+      <c r="D33" s="47"/>
       <c r="E33" s="44"/>
       <c r="F33" s="45"/>
     </row>
@@ -10642,7 +10659,7 @@
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="48"/>
+      <c r="D34" s="47"/>
       <c r="E34" s="44"/>
       <c r="F34" s="45"/>
     </row>
@@ -10652,7 +10669,7 @@
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="48"/>
+      <c r="D35" s="47"/>
       <c r="E35" s="44"/>
       <c r="F35" s="45"/>
     </row>
@@ -10662,7 +10679,7 @@
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="48"/>
+      <c r="D36" s="47"/>
       <c r="E36" s="44"/>
       <c r="F36" s="45"/>
     </row>
@@ -10672,7 +10689,7 @@
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="48"/>
+      <c r="D37" s="47"/>
       <c r="E37" s="44"/>
       <c r="F37" s="45"/>
     </row>
@@ -10682,7 +10699,7 @@
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="48"/>
+      <c r="D38" s="47"/>
       <c r="E38" s="44"/>
       <c r="F38" s="45"/>
     </row>
@@ -10692,7 +10709,7 @@
       </c>
       <c r="B39" s="42"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="48"/>
+      <c r="D39" s="47"/>
       <c r="E39" s="44"/>
       <c r="F39" s="45"/>
     </row>
@@ -10702,7 +10719,7 @@
       </c>
       <c r="B40" s="42"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="48"/>
+      <c r="D40" s="47"/>
       <c r="E40" s="44"/>
       <c r="F40" s="45"/>
     </row>
@@ -10712,7 +10729,7 @@
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="48"/>
+      <c r="D41" s="47"/>
       <c r="E41" s="44"/>
       <c r="F41" s="45"/>
     </row>
@@ -10722,7 +10739,7 @@
       </c>
       <c r="B42" s="42"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="48"/>
+      <c r="D42" s="47"/>
       <c r="E42" s="44"/>
       <c r="F42" s="45"/>
     </row>
@@ -10732,7 +10749,7 @@
       </c>
       <c r="B43" s="42"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="48"/>
+      <c r="D43" s="47"/>
       <c r="E43" s="44"/>
       <c r="F43" s="45"/>
     </row>
@@ -10742,7 +10759,7 @@
       </c>
       <c r="B44" s="42"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="48"/>
+      <c r="D44" s="47"/>
       <c r="E44" s="44"/>
       <c r="F44" s="45"/>
     </row>
@@ -10752,7 +10769,7 @@
       </c>
       <c r="B45" s="42"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="48"/>
+      <c r="D45" s="47"/>
       <c r="E45" s="44"/>
       <c r="F45" s="45"/>
     </row>
@@ -10762,7 +10779,7 @@
       </c>
       <c r="B46" s="42"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="48"/>
+      <c r="D46" s="47"/>
       <c r="E46" s="44"/>
       <c r="F46" s="45"/>
     </row>
@@ -10772,7 +10789,7 @@
       </c>
       <c r="B47" s="42"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="48"/>
+      <c r="D47" s="47"/>
       <c r="E47" s="44"/>
       <c r="F47" s="45"/>
     </row>
@@ -10782,7 +10799,7 @@
       </c>
       <c r="B48" s="42"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="48"/>
+      <c r="D48" s="47"/>
       <c r="E48" s="44"/>
       <c r="F48" s="45"/>
     </row>
@@ -10792,7 +10809,7 @@
       </c>
       <c r="B49" s="42"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="48"/>
+      <c r="D49" s="47"/>
       <c r="E49" s="44"/>
       <c r="F49" s="45"/>
     </row>
@@ -10802,7 +10819,7 @@
       </c>
       <c r="B50" s="42"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="48"/>
+      <c r="D50" s="47"/>
       <c r="E50" s="44"/>
       <c r="F50" s="45"/>
     </row>
@@ -10812,7 +10829,7 @@
       </c>
       <c r="B51" s="42"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="48"/>
+      <c r="D51" s="47"/>
       <c r="E51" s="44"/>
       <c r="F51" s="45"/>
     </row>
@@ -10822,7 +10839,7 @@
       </c>
       <c r="B52" s="42"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="48"/>
+      <c r="D52" s="47"/>
       <c r="E52" s="44"/>
       <c r="F52" s="45"/>
     </row>
@@ -10832,7 +10849,7 @@
       </c>
       <c r="B53" s="42"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="48"/>
+      <c r="D53" s="47"/>
       <c r="E53" s="44"/>
       <c r="F53" s="45"/>
     </row>
@@ -10842,7 +10859,7 @@
       </c>
       <c r="B54" s="42"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="48"/>
+      <c r="D54" s="47"/>
       <c r="E54" s="44"/>
       <c r="F54" s="45"/>
     </row>
@@ -10852,7 +10869,7 @@
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="48"/>
+      <c r="D55" s="47"/>
       <c r="E55" s="44"/>
       <c r="F55" s="45"/>
     </row>
@@ -10862,7 +10879,7 @@
       </c>
       <c r="B56" s="42"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="48"/>
+      <c r="D56" s="47"/>
       <c r="E56" s="44"/>
       <c r="F56" s="45"/>
     </row>
@@ -10872,7 +10889,7 @@
       </c>
       <c r="B57" s="42"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="48"/>
+      <c r="D57" s="47"/>
       <c r="E57" s="44"/>
       <c r="F57" s="45"/>
     </row>
@@ -10882,7 +10899,7 @@
       </c>
       <c r="B58" s="42"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="48"/>
+      <c r="D58" s="47"/>
       <c r="E58" s="44"/>
       <c r="F58" s="45"/>
     </row>
@@ -10892,7 +10909,7 @@
       </c>
       <c r="B59" s="42"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="48"/>
+      <c r="D59" s="47"/>
       <c r="E59" s="44"/>
       <c r="F59" s="45"/>
     </row>
@@ -10902,7 +10919,7 @@
       </c>
       <c r="B60" s="42"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="48"/>
+      <c r="D60" s="47"/>
       <c r="E60" s="44"/>
       <c r="F60" s="45"/>
     </row>
@@ -10912,7 +10929,7 @@
       </c>
       <c r="B61" s="42"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="48"/>
+      <c r="D61" s="47"/>
       <c r="E61" s="44"/>
       <c r="F61" s="45"/>
     </row>
@@ -10922,7 +10939,7 @@
       </c>
       <c r="B62" s="42"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="48"/>
+      <c r="D62" s="47"/>
       <c r="E62" s="44"/>
       <c r="F62" s="45"/>
     </row>
@@ -10932,7 +10949,7 @@
       </c>
       <c r="B63" s="42"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="48"/>
+      <c r="D63" s="47"/>
       <c r="E63" s="44"/>
       <c r="F63" s="45"/>
     </row>
@@ -10942,7 +10959,7 @@
       </c>
       <c r="B64" s="42"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="48"/>
+      <c r="D64" s="47"/>
       <c r="E64" s="44"/>
       <c r="F64" s="45"/>
     </row>
@@ -10952,7 +10969,7 @@
       </c>
       <c r="B65" s="42"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="48"/>
+      <c r="D65" s="47"/>
       <c r="E65" s="44"/>
       <c r="F65" s="45"/>
     </row>
@@ -10962,7 +10979,7 @@
       </c>
       <c r="B66" s="42"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="48"/>
+      <c r="D66" s="47"/>
       <c r="E66" s="44"/>
       <c r="F66" s="45"/>
     </row>
@@ -10972,7 +10989,7 @@
       </c>
       <c r="B67" s="42"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="48"/>
+      <c r="D67" s="47"/>
       <c r="E67" s="44"/>
       <c r="F67" s="45"/>
     </row>
@@ -10982,7 +10999,7 @@
       </c>
       <c r="B68" s="42"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="48"/>
+      <c r="D68" s="47"/>
       <c r="E68" s="44"/>
       <c r="F68" s="45"/>
     </row>
@@ -10992,7 +11009,7 @@
       </c>
       <c r="B69" s="42"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="48"/>
+      <c r="D69" s="47"/>
       <c r="E69" s="44"/>
       <c r="F69" s="45"/>
     </row>
@@ -11002,7 +11019,7 @@
       </c>
       <c r="B70" s="42"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="48"/>
+      <c r="D70" s="47"/>
       <c r="E70" s="44"/>
       <c r="F70" s="45"/>
     </row>
@@ -11012,7 +11029,7 @@
       </c>
       <c r="B71" s="42"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="48"/>
+      <c r="D71" s="47"/>
       <c r="E71" s="44"/>
       <c r="F71" s="45"/>
     </row>
@@ -11022,7 +11039,7 @@
       </c>
       <c r="B72" s="42"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="48"/>
+      <c r="D72" s="47"/>
       <c r="E72" s="44"/>
       <c r="F72" s="45"/>
     </row>
@@ -11032,7 +11049,7 @@
       </c>
       <c r="B73" s="42"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="48"/>
+      <c r="D73" s="47"/>
       <c r="E73" s="44"/>
       <c r="F73" s="45"/>
     </row>
@@ -11042,7 +11059,7 @@
       </c>
       <c r="B74" s="42"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="48"/>
+      <c r="D74" s="47"/>
       <c r="E74" s="44"/>
       <c r="F74" s="45"/>
     </row>
@@ -11052,7 +11069,7 @@
       </c>
       <c r="B75" s="42"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="48"/>
+      <c r="D75" s="47"/>
       <c r="E75" s="44"/>
       <c r="F75" s="45"/>
     </row>
@@ -11062,7 +11079,7 @@
       </c>
       <c r="B76" s="42"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="48"/>
+      <c r="D76" s="47"/>
       <c r="E76" s="44"/>
       <c r="F76" s="45"/>
     </row>
@@ -11072,7 +11089,7 @@
       </c>
       <c r="B77" s="42"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="48"/>
+      <c r="D77" s="47"/>
       <c r="E77" s="44"/>
       <c r="F77" s="45"/>
     </row>
@@ -11082,7 +11099,7 @@
       </c>
       <c r="B78" s="42"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="48"/>
+      <c r="D78" s="47"/>
       <c r="E78" s="44"/>
       <c r="F78" s="45"/>
     </row>
@@ -11092,7 +11109,7 @@
       </c>
       <c r="B79" s="42"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="48"/>
+      <c r="D79" s="47"/>
       <c r="E79" s="44"/>
       <c r="F79" s="45"/>
     </row>
@@ -11102,7 +11119,7 @@
       </c>
       <c r="B80" s="42"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="48"/>
+      <c r="D80" s="47"/>
       <c r="E80" s="44"/>
       <c r="F80" s="45"/>
     </row>
@@ -11112,7 +11129,7 @@
       </c>
       <c r="B81" s="42"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="48"/>
+      <c r="D81" s="47"/>
       <c r="E81" s="44"/>
       <c r="F81" s="45"/>
     </row>
@@ -11122,7 +11139,7 @@
       </c>
       <c r="B82" s="42"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="48"/>
+      <c r="D82" s="47"/>
       <c r="E82" s="44"/>
       <c r="F82" s="45"/>
     </row>
@@ -11132,7 +11149,7 @@
       </c>
       <c r="B83" s="42"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="48"/>
+      <c r="D83" s="47"/>
       <c r="E83" s="44"/>
       <c r="F83" s="45"/>
     </row>
@@ -11142,7 +11159,7 @@
       </c>
       <c r="B84" s="42"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="48"/>
+      <c r="D84" s="47"/>
       <c r="E84" s="44"/>
       <c r="F84" s="45"/>
     </row>
@@ -11152,7 +11169,7 @@
       </c>
       <c r="B85" s="42"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="48"/>
+      <c r="D85" s="47"/>
       <c r="E85" s="44"/>
       <c r="F85" s="45"/>
     </row>
@@ -11162,7 +11179,7 @@
       </c>
       <c r="B86" s="42"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="48"/>
+      <c r="D86" s="47"/>
       <c r="E86" s="44"/>
       <c r="F86" s="45"/>
     </row>
@@ -11172,7 +11189,7 @@
       </c>
       <c r="B87" s="42"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="48"/>
+      <c r="D87" s="47"/>
       <c r="E87" s="44"/>
       <c r="F87" s="45"/>
     </row>
@@ -11182,7 +11199,7 @@
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="48"/>
+      <c r="D88" s="47"/>
       <c r="E88" s="44"/>
       <c r="F88" s="45"/>
     </row>
@@ -11192,7 +11209,7 @@
       </c>
       <c r="B89" s="42"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="48"/>
+      <c r="D89" s="47"/>
       <c r="E89" s="44"/>
       <c r="F89" s="45"/>
     </row>
@@ -11202,7 +11219,7 @@
       </c>
       <c r="B90" s="42"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="48"/>
+      <c r="D90" s="47"/>
       <c r="E90" s="44"/>
       <c r="F90" s="45"/>
     </row>
@@ -11212,7 +11229,7 @@
       </c>
       <c r="B91" s="42"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="48"/>
+      <c r="D91" s="47"/>
       <c r="E91" s="44"/>
       <c r="F91" s="45"/>
     </row>
@@ -11222,7 +11239,7 @@
       </c>
       <c r="B92" s="42"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="48"/>
+      <c r="D92" s="47"/>
       <c r="E92" s="44"/>
       <c r="F92" s="45"/>
     </row>
@@ -11232,7 +11249,7 @@
       </c>
       <c r="B93" s="42"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="48"/>
+      <c r="D93" s="47"/>
       <c r="E93" s="44"/>
       <c r="F93" s="45"/>
     </row>
@@ -11242,7 +11259,7 @@
       </c>
       <c r="B94" s="42"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="48"/>
+      <c r="D94" s="47"/>
       <c r="E94" s="44"/>
       <c r="F94" s="45"/>
     </row>
@@ -11252,7 +11269,7 @@
       </c>
       <c r="B95" s="42"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="48"/>
+      <c r="D95" s="47"/>
       <c r="E95" s="44"/>
       <c r="F95" s="45"/>
     </row>
@@ -11262,7 +11279,7 @@
       </c>
       <c r="B96" s="42"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="48"/>
+      <c r="D96" s="47"/>
       <c r="E96" s="44"/>
       <c r="F96" s="45"/>
     </row>
@@ -11272,7 +11289,7 @@
       </c>
       <c r="B97" s="42"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="48"/>
+      <c r="D97" s="47"/>
       <c r="E97" s="44"/>
       <c r="F97" s="45"/>
     </row>
@@ -11282,7 +11299,7 @@
       </c>
       <c r="B98" s="42"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="48"/>
+      <c r="D98" s="47"/>
       <c r="E98" s="44"/>
       <c r="F98" s="45"/>
     </row>
@@ -11292,7 +11309,7 @@
       </c>
       <c r="B99" s="42"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="48"/>
+      <c r="D99" s="47"/>
       <c r="E99" s="44"/>
       <c r="F99" s="45"/>
     </row>
@@ -11302,7 +11319,7 @@
       </c>
       <c r="B100" s="42"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="48"/>
+      <c r="D100" s="47"/>
       <c r="E100" s="44"/>
       <c r="F100" s="45"/>
     </row>
@@ -11355,7 +11372,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -11372,8 +11389,8 @@
         <f aca="false">'Sprint 05 Backlog'!B1+1</f>
         <v>6</v>
       </c>
-      <c r="C1" s="49" t="s">
-        <v>193</v>
+      <c r="C1" s="48" t="s">
+        <v>195</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>2</v>
@@ -11569,8 +11586,8 @@
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
-      <c r="D15" s="49" t="s">
-        <v>194</v>
+      <c r="D15" s="48" t="s">
+        <v>196</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>
@@ -11613,7 +11630,7 @@
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="48"/>
+      <c r="D18" s="47"/>
       <c r="E18" s="44"/>
       <c r="F18" s="45"/>
     </row>
@@ -11623,7 +11640,7 @@
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="48"/>
+      <c r="D19" s="47"/>
       <c r="E19" s="44"/>
       <c r="F19" s="45"/>
     </row>
@@ -11633,7 +11650,7 @@
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="48"/>
+      <c r="D20" s="47"/>
       <c r="E20" s="44"/>
       <c r="F20" s="45"/>
     </row>
@@ -11643,7 +11660,7 @@
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="48"/>
+      <c r="D21" s="47"/>
       <c r="E21" s="44"/>
       <c r="F21" s="45"/>
     </row>
@@ -11653,7 +11670,7 @@
       </c>
       <c r="B22" s="42"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="48"/>
+      <c r="D22" s="47"/>
       <c r="E22" s="44"/>
       <c r="F22" s="45"/>
     </row>
@@ -11663,7 +11680,7 @@
       </c>
       <c r="B23" s="42"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="48"/>
+      <c r="D23" s="47"/>
       <c r="E23" s="44"/>
       <c r="F23" s="45"/>
     </row>
@@ -11673,7 +11690,7 @@
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="48"/>
+      <c r="D24" s="47"/>
       <c r="E24" s="44"/>
       <c r="F24" s="45"/>
     </row>
@@ -11683,7 +11700,7 @@
       </c>
       <c r="B25" s="42"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="48"/>
+      <c r="D25" s="47"/>
       <c r="E25" s="44"/>
       <c r="F25" s="45"/>
     </row>
@@ -11693,7 +11710,7 @@
       </c>
       <c r="B26" s="42"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="48"/>
+      <c r="D26" s="47"/>
       <c r="E26" s="44"/>
       <c r="F26" s="45"/>
     </row>
@@ -11703,7 +11720,7 @@
       </c>
       <c r="B27" s="42"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="48"/>
+      <c r="D27" s="47"/>
       <c r="E27" s="44"/>
       <c r="F27" s="45"/>
     </row>
@@ -11713,7 +11730,7 @@
       </c>
       <c r="B28" s="42"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="48"/>
+      <c r="D28" s="47"/>
       <c r="E28" s="44"/>
       <c r="F28" s="45"/>
     </row>
@@ -11723,7 +11740,7 @@
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="48"/>
+      <c r="D29" s="47"/>
       <c r="E29" s="44"/>
       <c r="F29" s="45"/>
     </row>
@@ -11733,7 +11750,7 @@
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="48"/>
+      <c r="D30" s="47"/>
       <c r="E30" s="44"/>
       <c r="F30" s="45"/>
     </row>
@@ -11743,7 +11760,7 @@
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="48"/>
+      <c r="D31" s="47"/>
       <c r="E31" s="44"/>
       <c r="F31" s="45"/>
     </row>
@@ -11753,7 +11770,7 @@
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="48"/>
+      <c r="D32" s="47"/>
       <c r="E32" s="44"/>
       <c r="F32" s="45"/>
     </row>
@@ -11763,7 +11780,7 @@
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="48"/>
+      <c r="D33" s="47"/>
       <c r="E33" s="44"/>
       <c r="F33" s="45"/>
     </row>
@@ -11773,7 +11790,7 @@
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="48"/>
+      <c r="D34" s="47"/>
       <c r="E34" s="44"/>
       <c r="F34" s="45"/>
     </row>
@@ -11783,7 +11800,7 @@
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="48"/>
+      <c r="D35" s="47"/>
       <c r="E35" s="44"/>
       <c r="F35" s="45"/>
     </row>
@@ -11793,7 +11810,7 @@
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="48"/>
+      <c r="D36" s="47"/>
       <c r="E36" s="44"/>
       <c r="F36" s="45"/>
     </row>
@@ -11803,7 +11820,7 @@
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="48"/>
+      <c r="D37" s="47"/>
       <c r="E37" s="44"/>
       <c r="F37" s="45"/>
     </row>
@@ -11813,7 +11830,7 @@
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="48"/>
+      <c r="D38" s="47"/>
       <c r="E38" s="44"/>
       <c r="F38" s="45"/>
     </row>
@@ -11823,7 +11840,7 @@
       </c>
       <c r="B39" s="42"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="48"/>
+      <c r="D39" s="47"/>
       <c r="E39" s="44"/>
       <c r="F39" s="45"/>
     </row>
@@ -11833,7 +11850,7 @@
       </c>
       <c r="B40" s="42"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="48"/>
+      <c r="D40" s="47"/>
       <c r="E40" s="44"/>
       <c r="F40" s="45"/>
     </row>
@@ -11843,7 +11860,7 @@
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="48"/>
+      <c r="D41" s="47"/>
       <c r="E41" s="44"/>
       <c r="F41" s="45"/>
     </row>
@@ -11853,7 +11870,7 @@
       </c>
       <c r="B42" s="42"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="48"/>
+      <c r="D42" s="47"/>
       <c r="E42" s="44"/>
       <c r="F42" s="45"/>
     </row>
@@ -11863,7 +11880,7 @@
       </c>
       <c r="B43" s="42"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="48"/>
+      <c r="D43" s="47"/>
       <c r="E43" s="44"/>
       <c r="F43" s="45"/>
     </row>
@@ -11873,7 +11890,7 @@
       </c>
       <c r="B44" s="42"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="48"/>
+      <c r="D44" s="47"/>
       <c r="E44" s="44"/>
       <c r="F44" s="45"/>
     </row>
@@ -11883,7 +11900,7 @@
       </c>
       <c r="B45" s="42"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="48"/>
+      <c r="D45" s="47"/>
       <c r="E45" s="44"/>
       <c r="F45" s="45"/>
     </row>
@@ -11893,7 +11910,7 @@
       </c>
       <c r="B46" s="42"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="48"/>
+      <c r="D46" s="47"/>
       <c r="E46" s="44"/>
       <c r="F46" s="45"/>
     </row>
@@ -11903,7 +11920,7 @@
       </c>
       <c r="B47" s="42"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="48"/>
+      <c r="D47" s="47"/>
       <c r="E47" s="44"/>
       <c r="F47" s="45"/>
     </row>
@@ -11913,7 +11930,7 @@
       </c>
       <c r="B48" s="42"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="48"/>
+      <c r="D48" s="47"/>
       <c r="E48" s="44"/>
       <c r="F48" s="45"/>
     </row>
@@ -11923,7 +11940,7 @@
       </c>
       <c r="B49" s="42"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="48"/>
+      <c r="D49" s="47"/>
       <c r="E49" s="44"/>
       <c r="F49" s="45"/>
     </row>
@@ -11933,7 +11950,7 @@
       </c>
       <c r="B50" s="42"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="48"/>
+      <c r="D50" s="47"/>
       <c r="E50" s="44"/>
       <c r="F50" s="45"/>
     </row>
@@ -11943,7 +11960,7 @@
       </c>
       <c r="B51" s="42"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="48"/>
+      <c r="D51" s="47"/>
       <c r="E51" s="44"/>
       <c r="F51" s="45"/>
     </row>
@@ -11953,7 +11970,7 @@
       </c>
       <c r="B52" s="42"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="48"/>
+      <c r="D52" s="47"/>
       <c r="E52" s="44"/>
       <c r="F52" s="45"/>
     </row>
@@ -11963,7 +11980,7 @@
       </c>
       <c r="B53" s="42"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="48"/>
+      <c r="D53" s="47"/>
       <c r="E53" s="44"/>
       <c r="F53" s="45"/>
     </row>
@@ -11973,7 +11990,7 @@
       </c>
       <c r="B54" s="42"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="48"/>
+      <c r="D54" s="47"/>
       <c r="E54" s="44"/>
       <c r="F54" s="45"/>
     </row>
@@ -11983,7 +12000,7 @@
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="48"/>
+      <c r="D55" s="47"/>
       <c r="E55" s="44"/>
       <c r="F55" s="45"/>
     </row>
@@ -11993,7 +12010,7 @@
       </c>
       <c r="B56" s="42"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="48"/>
+      <c r="D56" s="47"/>
       <c r="E56" s="44"/>
       <c r="F56" s="45"/>
     </row>
@@ -12003,7 +12020,7 @@
       </c>
       <c r="B57" s="42"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="48"/>
+      <c r="D57" s="47"/>
       <c r="E57" s="44"/>
       <c r="F57" s="45"/>
     </row>
@@ -12013,7 +12030,7 @@
       </c>
       <c r="B58" s="42"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="48"/>
+      <c r="D58" s="47"/>
       <c r="E58" s="44"/>
       <c r="F58" s="45"/>
     </row>
@@ -12023,7 +12040,7 @@
       </c>
       <c r="B59" s="42"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="48"/>
+      <c r="D59" s="47"/>
       <c r="E59" s="44"/>
       <c r="F59" s="45"/>
     </row>
@@ -12033,7 +12050,7 @@
       </c>
       <c r="B60" s="42"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="48"/>
+      <c r="D60" s="47"/>
       <c r="E60" s="44"/>
       <c r="F60" s="45"/>
     </row>
@@ -12043,7 +12060,7 @@
       </c>
       <c r="B61" s="42"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="48"/>
+      <c r="D61" s="47"/>
       <c r="E61" s="44"/>
       <c r="F61" s="45"/>
     </row>
@@ -12053,7 +12070,7 @@
       </c>
       <c r="B62" s="42"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="48"/>
+      <c r="D62" s="47"/>
       <c r="E62" s="44"/>
       <c r="F62" s="45"/>
     </row>
@@ -12063,7 +12080,7 @@
       </c>
       <c r="B63" s="42"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="48"/>
+      <c r="D63" s="47"/>
       <c r="E63" s="44"/>
       <c r="F63" s="45"/>
     </row>
@@ -12073,7 +12090,7 @@
       </c>
       <c r="B64" s="42"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="48"/>
+      <c r="D64" s="47"/>
       <c r="E64" s="44"/>
       <c r="F64" s="45"/>
     </row>
@@ -12083,7 +12100,7 @@
       </c>
       <c r="B65" s="42"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="48"/>
+      <c r="D65" s="47"/>
       <c r="E65" s="44"/>
       <c r="F65" s="45"/>
     </row>
@@ -12093,7 +12110,7 @@
       </c>
       <c r="B66" s="42"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="48"/>
+      <c r="D66" s="47"/>
       <c r="E66" s="44"/>
       <c r="F66" s="45"/>
     </row>
@@ -12103,7 +12120,7 @@
       </c>
       <c r="B67" s="42"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="48"/>
+      <c r="D67" s="47"/>
       <c r="E67" s="44"/>
       <c r="F67" s="45"/>
     </row>
@@ -12113,7 +12130,7 @@
       </c>
       <c r="B68" s="42"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="48"/>
+      <c r="D68" s="47"/>
       <c r="E68" s="44"/>
       <c r="F68" s="45"/>
     </row>
@@ -12123,7 +12140,7 @@
       </c>
       <c r="B69" s="42"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="48"/>
+      <c r="D69" s="47"/>
       <c r="E69" s="44"/>
       <c r="F69" s="45"/>
     </row>
@@ -12133,7 +12150,7 @@
       </c>
       <c r="B70" s="42"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="48"/>
+      <c r="D70" s="47"/>
       <c r="E70" s="44"/>
       <c r="F70" s="45"/>
     </row>
@@ -12143,7 +12160,7 @@
       </c>
       <c r="B71" s="42"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="48"/>
+      <c r="D71" s="47"/>
       <c r="E71" s="44"/>
       <c r="F71" s="45"/>
     </row>
@@ -12153,7 +12170,7 @@
       </c>
       <c r="B72" s="42"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="48"/>
+      <c r="D72" s="47"/>
       <c r="E72" s="44"/>
       <c r="F72" s="45"/>
     </row>
@@ -12163,7 +12180,7 @@
       </c>
       <c r="B73" s="42"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="48"/>
+      <c r="D73" s="47"/>
       <c r="E73" s="44"/>
       <c r="F73" s="45"/>
     </row>
@@ -12173,7 +12190,7 @@
       </c>
       <c r="B74" s="42"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="48"/>
+      <c r="D74" s="47"/>
       <c r="E74" s="44"/>
       <c r="F74" s="45"/>
     </row>
@@ -12183,7 +12200,7 @@
       </c>
       <c r="B75" s="42"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="48"/>
+      <c r="D75" s="47"/>
       <c r="E75" s="44"/>
       <c r="F75" s="45"/>
     </row>
@@ -12193,7 +12210,7 @@
       </c>
       <c r="B76" s="42"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="48"/>
+      <c r="D76" s="47"/>
       <c r="E76" s="44"/>
       <c r="F76" s="45"/>
     </row>
@@ -12203,7 +12220,7 @@
       </c>
       <c r="B77" s="42"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="48"/>
+      <c r="D77" s="47"/>
       <c r="E77" s="44"/>
       <c r="F77" s="45"/>
     </row>
@@ -12213,7 +12230,7 @@
       </c>
       <c r="B78" s="42"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="48"/>
+      <c r="D78" s="47"/>
       <c r="E78" s="44"/>
       <c r="F78" s="45"/>
     </row>
@@ -12223,7 +12240,7 @@
       </c>
       <c r="B79" s="42"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="48"/>
+      <c r="D79" s="47"/>
       <c r="E79" s="44"/>
       <c r="F79" s="45"/>
     </row>
@@ -12233,7 +12250,7 @@
       </c>
       <c r="B80" s="42"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="48"/>
+      <c r="D80" s="47"/>
       <c r="E80" s="44"/>
       <c r="F80" s="45"/>
     </row>
@@ -12243,7 +12260,7 @@
       </c>
       <c r="B81" s="42"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="48"/>
+      <c r="D81" s="47"/>
       <c r="E81" s="44"/>
       <c r="F81" s="45"/>
     </row>
@@ -12253,7 +12270,7 @@
       </c>
       <c r="B82" s="42"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="48"/>
+      <c r="D82" s="47"/>
       <c r="E82" s="44"/>
       <c r="F82" s="45"/>
     </row>
@@ -12263,7 +12280,7 @@
       </c>
       <c r="B83" s="42"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="48"/>
+      <c r="D83" s="47"/>
       <c r="E83" s="44"/>
       <c r="F83" s="45"/>
     </row>
@@ -12273,7 +12290,7 @@
       </c>
       <c r="B84" s="42"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="48"/>
+      <c r="D84" s="47"/>
       <c r="E84" s="44"/>
       <c r="F84" s="45"/>
     </row>
@@ -12283,7 +12300,7 @@
       </c>
       <c r="B85" s="42"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="48"/>
+      <c r="D85" s="47"/>
       <c r="E85" s="44"/>
       <c r="F85" s="45"/>
     </row>
@@ -12293,7 +12310,7 @@
       </c>
       <c r="B86" s="42"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="48"/>
+      <c r="D86" s="47"/>
       <c r="E86" s="44"/>
       <c r="F86" s="45"/>
     </row>
@@ -12303,7 +12320,7 @@
       </c>
       <c r="B87" s="42"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="48"/>
+      <c r="D87" s="47"/>
       <c r="E87" s="44"/>
       <c r="F87" s="45"/>
     </row>
@@ -12313,7 +12330,7 @@
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="48"/>
+      <c r="D88" s="47"/>
       <c r="E88" s="44"/>
       <c r="F88" s="45"/>
     </row>
@@ -12323,7 +12340,7 @@
       </c>
       <c r="B89" s="42"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="48"/>
+      <c r="D89" s="47"/>
       <c r="E89" s="44"/>
       <c r="F89" s="45"/>
     </row>
@@ -12333,7 +12350,7 @@
       </c>
       <c r="B90" s="42"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="48"/>
+      <c r="D90" s="47"/>
       <c r="E90" s="44"/>
       <c r="F90" s="45"/>
     </row>
@@ -12343,7 +12360,7 @@
       </c>
       <c r="B91" s="42"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="48"/>
+      <c r="D91" s="47"/>
       <c r="E91" s="44"/>
       <c r="F91" s="45"/>
     </row>
@@ -12353,7 +12370,7 @@
       </c>
       <c r="B92" s="42"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="48"/>
+      <c r="D92" s="47"/>
       <c r="E92" s="44"/>
       <c r="F92" s="45"/>
     </row>
@@ -12363,7 +12380,7 @@
       </c>
       <c r="B93" s="42"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="48"/>
+      <c r="D93" s="47"/>
       <c r="E93" s="44"/>
       <c r="F93" s="45"/>
     </row>
@@ -12373,7 +12390,7 @@
       </c>
       <c r="B94" s="42"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="48"/>
+      <c r="D94" s="47"/>
       <c r="E94" s="44"/>
       <c r="F94" s="45"/>
     </row>
@@ -12383,7 +12400,7 @@
       </c>
       <c r="B95" s="42"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="48"/>
+      <c r="D95" s="47"/>
       <c r="E95" s="44"/>
       <c r="F95" s="45"/>
     </row>
@@ -12393,7 +12410,7 @@
       </c>
       <c r="B96" s="42"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="48"/>
+      <c r="D96" s="47"/>
       <c r="E96" s="44"/>
       <c r="F96" s="45"/>
     </row>
@@ -12403,7 +12420,7 @@
       </c>
       <c r="B97" s="42"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="48"/>
+      <c r="D97" s="47"/>
       <c r="E97" s="44"/>
       <c r="F97" s="45"/>
     </row>
@@ -12413,7 +12430,7 @@
       </c>
       <c r="B98" s="42"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="48"/>
+      <c r="D98" s="47"/>
       <c r="E98" s="44"/>
       <c r="F98" s="45"/>
     </row>
@@ -12423,7 +12440,7 @@
       </c>
       <c r="B99" s="42"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="48"/>
+      <c r="D99" s="47"/>
       <c r="E99" s="44"/>
       <c r="F99" s="45"/>
     </row>
@@ -12433,7 +12450,7 @@
       </c>
       <c r="B100" s="42"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="48"/>
+      <c r="D100" s="47"/>
       <c r="E100" s="44"/>
       <c r="F100" s="45"/>
     </row>

</xml_diff>

<commit_message>
P07 Load (File > Open) 3/19/2023 5:37 PM
</commit_message>
<xml_diff>
--- a/P07/Scrum_Sprint_3.xlsx
+++ b/P07/Scrum_Sprint_3.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="202">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -611,6 +611,62 @@
   </si>
   <si>
     <t xml:space="preserve">git commit -m "P07 Save/Load Option 3/17/2023 1:15 PM"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git commit -m "P07 Save/Load Order  3/18/2023 1:15 AM"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save (via method) &amp; reload (via constructor) each obj. Store &amp; Order </t>
+  </si>
+  <si>
+    <t xml:space="preserve">git commit -m "P07 Save/Load Order  3/19/2023 2:37 AM"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Write - “l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">oad” data form a specified file (File &gt; Open)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Add</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (File &gt; Open)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to GitHub</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">BONUS</t>
@@ -628,7 +684,7 @@
     <numFmt numFmtId="165" formatCode="mmm\ dd"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -734,6 +790,11 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1102,7 +1163,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1148,10 +1209,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.082244859696269"/>
-          <c:y val="0.161931103847121"/>
-          <c:w val="0.884069745640897"/>
-          <c:h val="0.635403570530551"/>
+          <c:x val="0.08225"/>
+          <c:y val="0.161951464856029"/>
+          <c:w val="0.884"/>
+          <c:h val="0.635357726644034"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1241,24 +1302,24 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="99758733"/>
-        <c:axId val="90488292"/>
+        <c:axId val="52020894"/>
+        <c:axId val="96275871"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99758733"/>
+        <c:axId val="52020894"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1326,12 +1387,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90488292"/>
+        <c:crossAx val="96275871"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90488292"/>
+        <c:axId val="96275871"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1408,7 +1469,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99758733"/>
+        <c:crossAx val="52020894"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1435,7 +1496,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1563,11 +1624,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="29661122"/>
-        <c:axId val="53172241"/>
+        <c:axId val="2549610"/>
+        <c:axId val="65926684"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="29661122"/>
+        <c:axId val="2549610"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1633,7 +1694,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53172241"/>
+        <c:crossAx val="65926684"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1641,7 +1702,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53172241"/>
+        <c:axId val="65926684"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1717,7 +1778,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29661122"/>
+        <c:crossAx val="2549610"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1744,7 +1805,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1872,11 +1933,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="68411361"/>
-        <c:axId val="21569018"/>
+        <c:axId val="1611474"/>
+        <c:axId val="72009770"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68411361"/>
+        <c:axId val="1611474"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1942,7 +2003,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21569018"/>
+        <c:crossAx val="72009770"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1950,7 +2011,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="21569018"/>
+        <c:axId val="72009770"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2026,7 +2087,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68411361"/>
+        <c:crossAx val="1611474"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2053,7 +2114,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2145,28 +2206,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2181,11 +2242,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="13889259"/>
-        <c:axId val="76327102"/>
+        <c:axId val="22233120"/>
+        <c:axId val="73649646"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="13889259"/>
+        <c:axId val="22233120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2251,7 +2312,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76327102"/>
+        <c:crossAx val="73649646"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2259,7 +2320,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76327102"/>
+        <c:axId val="73649646"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2335,7 +2396,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13889259"/>
+        <c:crossAx val="22233120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2362,7 +2423,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2490,11 +2551,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="28573326"/>
-        <c:axId val="81280412"/>
+        <c:axId val="9511314"/>
+        <c:axId val="24524053"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="28573326"/>
+        <c:axId val="9511314"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2560,7 +2621,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81280412"/>
+        <c:crossAx val="24524053"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2568,7 +2629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81280412"/>
+        <c:axId val="24524053"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2644,7 +2705,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28573326"/>
+        <c:crossAx val="9511314"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2671,7 +2732,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2799,11 +2860,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="32991939"/>
-        <c:axId val="58960274"/>
+        <c:axId val="55888999"/>
+        <c:axId val="9504521"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="32991939"/>
+        <c:axId val="55888999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2869,7 +2930,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58960274"/>
+        <c:crossAx val="9504521"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2877,7 +2938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58960274"/>
+        <c:axId val="9504521"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2953,7 +3014,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32991939"/>
+        <c:crossAx val="55888999"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2980,7 +3041,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3108,11 +3169,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="72057821"/>
-        <c:axId val="68008980"/>
+        <c:axId val="62188440"/>
+        <c:axId val="67444079"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72057821"/>
+        <c:axId val="62188440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3178,7 +3239,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68008980"/>
+        <c:crossAx val="67444079"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3186,7 +3247,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68008980"/>
+        <c:axId val="67444079"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3262,7 +3323,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72057821"/>
+        <c:crossAx val="62188440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3300,9 +3361,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1904040</xdr:colOff>
+      <xdr:colOff>1903680</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>118800</xdr:rowOff>
+      <xdr:rowOff>118440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3310,8 +3371,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9123120" y="275040"/>
-        <a:ext cx="5760000" cy="2863080"/>
+        <a:off x="9122760" y="275040"/>
+        <a:ext cx="5759640" cy="2862720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3335,9 +3396,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1771560</xdr:colOff>
+      <xdr:colOff>1771200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3345,8 +3406,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="457920"/>
-        <a:ext cx="3751200" cy="1846440"/>
+        <a:off x="4092120" y="457920"/>
+        <a:ext cx="3750840" cy="1846080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3370,9 +3431,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>516960</xdr:colOff>
+      <xdr:colOff>516600</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3380,8 +3441,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="457920"/>
-        <a:ext cx="3746520" cy="1846440"/>
+        <a:off x="4092120" y="457920"/>
+        <a:ext cx="3745800" cy="1846080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3401,11 +3462,11 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>1679760</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>68040</xdr:rowOff>
+      <xdr:rowOff>68400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>516960</xdr:colOff>
+      <xdr:colOff>516600</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
@@ -3415,8 +3476,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="458280"/>
-        <a:ext cx="3746520" cy="1846440"/>
+        <a:off x="4092120" y="458640"/>
+        <a:ext cx="3745800" cy="1846080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3440,9 +3501,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>516960</xdr:colOff>
+      <xdr:colOff>516600</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3450,8 +3511,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="457920"/>
-        <a:ext cx="3746520" cy="1846440"/>
+        <a:off x="4092120" y="457920"/>
+        <a:ext cx="3745800" cy="1846080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3475,9 +3536,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>516960</xdr:colOff>
+      <xdr:colOff>516600</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3485,8 +3546,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="457920"/>
-        <a:ext cx="3746520" cy="1846440"/>
+        <a:off x="4092120" y="457920"/>
+        <a:ext cx="3745800" cy="1846080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3510,9 +3571,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>516960</xdr:colOff>
+      <xdr:colOff>516600</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3520,8 +3581,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="457920"/>
-        <a:ext cx="3746520" cy="1846440"/>
+        <a:off x="4092120" y="457920"/>
+        <a:ext cx="3745800" cy="1846080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3542,8 +3603,8 @@
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H34" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I40" activeCellId="0" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3553,8 +3614,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="36.99"/>
@@ -3787,11 +3848,11 @@
       </c>
       <c r="B15" s="3" t="n">
         <f aca="false">B14-C15</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C15" s="11" t="n">
         <f aca="false">COUNTIF(G$24:G$106,"Finished in Sprint 3")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="3"/>
@@ -3811,7 +3872,7 @@
       </c>
       <c r="B16" s="3" t="n">
         <f aca="false">B15-C16</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" s="11" t="n">
         <f aca="false">COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -3831,7 +3892,7 @@
       </c>
       <c r="B17" s="3" t="n">
         <f aca="false">B16-C17</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17" s="11" t="n">
         <f aca="false">COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4385,7 +4446,7 @@
         <v>3</v>
       </c>
       <c r="G37" s="21" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="H37" s="22" t="s">
         <v>86</v>
@@ -4484,7 +4545,7 @@
         <v>3</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="H40" s="22" t="s">
         <v>86</v>
@@ -5510,11 +5571,11 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -5980,7 +6041,7 @@
       </c>
       <c r="F30" s="45"/>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>15</v>
       </c>
@@ -6783,11 +6844,11 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -7946,11 +8007,11 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8039,7 +8100,7 @@
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -8052,7 +8113,7 @@
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">B7-C8</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C8" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -8068,7 +8129,7 @@
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">B8-C9</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C9" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -8084,7 +8145,7 @@
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">B9-C10</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C10" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -8100,11 +8161,11 @@
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">B10-C11</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C11" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32"/>
@@ -8116,11 +8177,11 @@
       </c>
       <c r="B12" s="32" t="n">
         <f aca="false">B11-C12</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C12" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
@@ -8132,7 +8193,7 @@
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">B12-C13</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C13" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -8148,7 +8209,7 @@
       </c>
       <c r="B14" s="32" t="n">
         <f aca="false">B13-C14</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C14" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -8244,7 +8305,7 @@
         <v>192</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="F20" s="45" t="s">
         <v>161</v>
@@ -8262,7 +8323,7 @@
         <v>193</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="F21" s="45"/>
     </row>
@@ -8296,61 +8357,97 @@
         <v>193</v>
       </c>
       <c r="E23" s="44" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="F23" s="45"/>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B24" s="42"/>
+      <c r="B24" s="42" t="s">
+        <v>85</v>
+      </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="45"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B25" s="42"/>
+      <c r="B25" s="42" t="s">
+        <v>85</v>
+      </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="44"/>
+      <c r="D25" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>81</v>
+      </c>
       <c r="F25" s="45"/>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B26" s="42"/>
+      <c r="B26" s="42" t="s">
+        <v>85</v>
+      </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="45"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="E26" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B27" s="42"/>
+      <c r="B27" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="44"/>
+      <c r="D27" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>81</v>
+      </c>
       <c r="F27" s="45"/>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B28" s="42"/>
+      <c r="B28" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="45"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="F28" s="45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>13</v>
       </c>
@@ -9071,12 +9168,16 @@
       <c r="F100" s="45"/>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="7">
+    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D28" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " promptTitle="Task ID" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A17:A100" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D18:D100" type="none">
+    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D18:D27 D29:D100" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9119,7 +9220,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -10245,7 +10346,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -11372,7 +11473,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -11390,7 +11491,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>2</v>
@@ -11587,7 +11688,7 @@
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="48" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>

</xml_diff>

<commit_message>
P07 Save (File > Save As) & (File > Save) 3/19/2023 9:10 PM
</commit_message>
<xml_diff>
--- a/P07/Scrum_Sprint_3.xlsx
+++ b/P07/Scrum_Sprint_3.xlsx
@@ -25,8 +25,58 @@
 </workbook>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="D28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">git commit -m "P07 Load (File &gt; Open) 3/19/2023 5:37 PM"
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">git commit -m "P07 Save (File &gt; Save As) 3/19/2023 9:10 PM"
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">git commit -m "P07 Save (File &gt; Save) 3/19/2023 9:10 PM"</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="206">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -629,7 +679,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Write - “l</t>
+      <t xml:space="preserve">Write – “L</t>
     </r>
     <r>
       <rPr>
@@ -667,6 +717,84 @@
       </rPr>
       <t xml:space="preserve"> to GitHub</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Write – “Save” data to a specified file (File &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Save As</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Add</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (File &gt; Save As)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to GitHub</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Finish write – “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Save” the data to a default file (File &gt; Save)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Add (File &gt; Save) to GitHub</t>
   </si>
   <si>
     <t xml:space="preserve">BONUS</t>
@@ -1163,7 +1291,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1302,24 +1430,24 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="52020894"/>
-        <c:axId val="96275871"/>
+        <c:axId val="10320767"/>
+        <c:axId val="16586463"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52020894"/>
+        <c:axId val="10320767"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1387,12 +1515,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96275871"/>
+        <c:crossAx val="16586463"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96275871"/>
+        <c:axId val="16586463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1469,7 +1597,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52020894"/>
+        <c:crossAx val="10320767"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1496,7 +1624,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart58.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1624,11 +1752,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="2549610"/>
-        <c:axId val="65926684"/>
+        <c:axId val="57197142"/>
+        <c:axId val="30071282"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2549610"/>
+        <c:axId val="57197142"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1694,7 +1822,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65926684"/>
+        <c:crossAx val="30071282"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1702,7 +1830,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65926684"/>
+        <c:axId val="30071282"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1778,7 +1906,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2549610"/>
+        <c:crossAx val="57197142"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1805,7 +1933,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart59.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1933,11 +2061,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="1611474"/>
-        <c:axId val="72009770"/>
+        <c:axId val="69295726"/>
+        <c:axId val="83495668"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1611474"/>
+        <c:axId val="69295726"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2003,7 +2131,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72009770"/>
+        <c:crossAx val="83495668"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2011,7 +2139,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72009770"/>
+        <c:axId val="83495668"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2087,7 +2215,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1611474"/>
+        <c:crossAx val="69295726"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2114,7 +2242,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart60.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2206,28 +2334,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2242,11 +2370,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="22233120"/>
-        <c:axId val="73649646"/>
+        <c:axId val="21366677"/>
+        <c:axId val="46196733"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="22233120"/>
+        <c:axId val="21366677"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2312,7 +2440,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73649646"/>
+        <c:crossAx val="46196733"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2320,7 +2448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73649646"/>
+        <c:axId val="46196733"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2396,7 +2524,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22233120"/>
+        <c:crossAx val="21366677"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2423,7 +2551,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart61.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2551,11 +2679,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="9511314"/>
-        <c:axId val="24524053"/>
+        <c:axId val="56854045"/>
+        <c:axId val="28232391"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="9511314"/>
+        <c:axId val="56854045"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2621,7 +2749,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24524053"/>
+        <c:crossAx val="28232391"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2629,7 +2757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="24524053"/>
+        <c:axId val="28232391"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2705,7 +2833,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9511314"/>
+        <c:crossAx val="56854045"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2732,7 +2860,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart62.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2860,11 +2988,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="55888999"/>
-        <c:axId val="9504521"/>
+        <c:axId val="77306003"/>
+        <c:axId val="86634760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55888999"/>
+        <c:axId val="77306003"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2930,7 +3058,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9504521"/>
+        <c:crossAx val="86634760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2938,7 +3066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9504521"/>
+        <c:axId val="86634760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3014,7 +3142,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55888999"/>
+        <c:crossAx val="77306003"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3041,7 +3169,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart63.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3169,11 +3297,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="62188440"/>
-        <c:axId val="67444079"/>
+        <c:axId val="92897935"/>
+        <c:axId val="29616921"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62188440"/>
+        <c:axId val="92897935"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3239,7 +3367,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67444079"/>
+        <c:crossAx val="29616921"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3247,7 +3375,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67444079"/>
+        <c:axId val="29616921"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3323,7 +3451,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62188440"/>
+        <c:crossAx val="92897935"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3604,7 +3732,7 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H34" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I40" activeCellId="0" sqref="I40"/>
+      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3848,11 +3976,11 @@
       </c>
       <c r="B15" s="3" t="n">
         <f aca="false">B14-C15</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="11" t="n">
         <f aca="false">COUNTIF(G$24:G$106,"Finished in Sprint 3")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="3"/>
@@ -3872,7 +4000,7 @@
       </c>
       <c r="B16" s="3" t="n">
         <f aca="false">B15-C16</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="11" t="n">
         <f aca="false">COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -3892,7 +4020,7 @@
       </c>
       <c r="B17" s="3" t="n">
         <f aca="false">B16-C17</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="11" t="n">
         <f aca="false">COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4512,7 +4640,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="21" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="H39" s="22" t="s">
         <v>86</v>
@@ -8007,8 +8135,8 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C22" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8100,7 +8228,7 @@
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -8113,7 +8241,7 @@
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">B7-C8</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C8" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -8129,7 +8257,7 @@
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">B8-C9</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -8145,7 +8273,7 @@
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">B9-C10</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C10" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -8161,7 +8289,7 @@
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">B10-C11</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C11" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -8177,11 +8305,11 @@
       </c>
       <c r="B12" s="32" t="n">
         <f aca="false">B11-C12</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C12" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
@@ -8193,7 +8321,7 @@
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">B12-C13</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -8209,7 +8337,7 @@
       </c>
       <c r="B14" s="32" t="n">
         <f aca="false">B13-C14</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -8451,41 +8579,65 @@
       <c r="A29" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B29" s="42"/>
+      <c r="B29" s="42" t="s">
+        <v>94</v>
+      </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="44"/>
+      <c r="D29" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="E29" s="44" t="s">
+        <v>81</v>
+      </c>
       <c r="F29" s="45"/>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B30" s="42"/>
+      <c r="B30" s="42" t="s">
+        <v>94</v>
+      </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="45"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D30" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="F30" s="45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="44"/>
+      <c r="D31" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>81</v>
+      </c>
       <c r="F31" s="45"/>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="45"/>
+      <c r="D32" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="F32" s="45" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -9169,7 +9321,7 @@
     </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D28" type="none">
+    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D28 D30" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9177,7 +9329,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D18:D27 D29:D100" type="none">
+    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D18:D27 D29 D31:D100" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9205,7 +9357,8 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -11491,7 +11644,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>2</v>
@@ -11688,7 +11841,7 @@
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="48" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>

</xml_diff>

<commit_message>
P07 Create a new, empty store 3/20/2023 3:15 PM
</commit_message>
<xml_diff>
--- a/P07/Scrum_Sprint_3.xlsx
+++ b/P07/Scrum_Sprint_3.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="206">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -927,7 +927,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -956,6 +956,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFAEAAAA"/>
         <bgColor rgb="FFB2B2B2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF420E"/>
       </patternFill>
     </fill>
   </fills>
@@ -1022,7 +1028,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1211,6 +1217,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1291,7 +1301,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart64.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1443,11 +1453,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="10320767"/>
-        <c:axId val="16586463"/>
+        <c:axId val="88963403"/>
+        <c:axId val="15607448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="10320767"/>
+        <c:axId val="88963403"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1515,12 +1525,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16586463"/>
+        <c:crossAx val="15607448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="16586463"/>
+        <c:axId val="15607448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1597,7 +1607,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10320767"/>
+        <c:crossAx val="88963403"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1624,7 +1634,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart65.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1752,11 +1762,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="57197142"/>
-        <c:axId val="30071282"/>
+        <c:axId val="80606315"/>
+        <c:axId val="91866000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57197142"/>
+        <c:axId val="80606315"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1822,7 +1832,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30071282"/>
+        <c:crossAx val="91866000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1830,7 +1840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30071282"/>
+        <c:axId val="91866000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1906,7 +1916,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57197142"/>
+        <c:crossAx val="80606315"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1933,7 +1943,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart66.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2061,11 +2071,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="69295726"/>
-        <c:axId val="83495668"/>
+        <c:axId val="94184479"/>
+        <c:axId val="3888204"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69295726"/>
+        <c:axId val="94184479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2131,7 +2141,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83495668"/>
+        <c:crossAx val="3888204"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2139,7 +2149,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83495668"/>
+        <c:axId val="3888204"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2215,7 +2225,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69295726"/>
+        <c:crossAx val="94184479"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2242,7 +2252,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart60.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart67.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2370,11 +2380,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="21366677"/>
-        <c:axId val="46196733"/>
+        <c:axId val="65140882"/>
+        <c:axId val="48166471"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="21366677"/>
+        <c:axId val="65140882"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2440,7 +2450,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46196733"/>
+        <c:crossAx val="48166471"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2448,7 +2458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46196733"/>
+        <c:axId val="48166471"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2524,7 +2534,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21366677"/>
+        <c:crossAx val="65140882"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2551,7 +2561,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart68.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2679,11 +2689,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="56854045"/>
-        <c:axId val="28232391"/>
+        <c:axId val="10863029"/>
+        <c:axId val="64564983"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56854045"/>
+        <c:axId val="10863029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2749,7 +2759,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28232391"/>
+        <c:crossAx val="64564983"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2757,7 +2767,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28232391"/>
+        <c:axId val="64564983"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2833,7 +2843,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56854045"/>
+        <c:crossAx val="10863029"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2860,7 +2870,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart69.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2988,11 +2998,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="77306003"/>
-        <c:axId val="86634760"/>
+        <c:axId val="23677773"/>
+        <c:axId val="98252033"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77306003"/>
+        <c:axId val="23677773"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3058,7 +3068,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86634760"/>
+        <c:crossAx val="98252033"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3066,7 +3076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86634760"/>
+        <c:axId val="98252033"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3142,7 +3152,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77306003"/>
+        <c:crossAx val="23677773"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3169,7 +3179,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart70.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3297,11 +3307,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="92897935"/>
-        <c:axId val="29616921"/>
+        <c:axId val="85645262"/>
+        <c:axId val="22886600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92897935"/>
+        <c:axId val="85645262"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3367,7 +3377,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29616921"/>
+        <c:crossAx val="22886600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3375,7 +3385,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29616921"/>
+        <c:axId val="22886600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3451,7 +3461,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92897935"/>
+        <c:crossAx val="85645262"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3731,8 +3741,8 @@
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H34" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8135,8 +8145,8 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C22" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8564,7 +8574,7 @@
       <c r="B28" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="47"/>
       <c r="D28" s="46" t="s">
         <v>199</v>
       </c>
@@ -8613,7 +8623,9 @@
       <c r="A31" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B31" s="42"/>
+      <c r="B31" s="42" t="s">
+        <v>85</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="46" t="s">
         <v>202</v>
@@ -9626,7 +9638,7 @@
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="47"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="44"/>
       <c r="F18" s="45"/>
     </row>
@@ -9636,7 +9648,7 @@
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="44"/>
       <c r="F19" s="45"/>
     </row>
@@ -9646,7 +9658,7 @@
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="44"/>
       <c r="F20" s="45"/>
     </row>
@@ -9656,7 +9668,7 @@
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="44"/>
       <c r="F21" s="45"/>
     </row>
@@ -9666,7 +9678,7 @@
       </c>
       <c r="B22" s="42"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="47"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="44"/>
       <c r="F22" s="45"/>
     </row>
@@ -9676,7 +9688,7 @@
       </c>
       <c r="B23" s="42"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="47"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="44"/>
       <c r="F23" s="45"/>
     </row>
@@ -9686,7 +9698,7 @@
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="47"/>
+      <c r="D24" s="48"/>
       <c r="E24" s="44"/>
       <c r="F24" s="45"/>
     </row>
@@ -9696,7 +9708,7 @@
       </c>
       <c r="B25" s="42"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="47"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="44"/>
       <c r="F25" s="45"/>
     </row>
@@ -9706,7 +9718,7 @@
       </c>
       <c r="B26" s="42"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="47"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="44"/>
       <c r="F26" s="45"/>
     </row>
@@ -9716,7 +9728,7 @@
       </c>
       <c r="B27" s="42"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="47"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="44"/>
       <c r="F27" s="45"/>
     </row>
@@ -9726,7 +9738,7 @@
       </c>
       <c r="B28" s="42"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="47"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="44"/>
       <c r="F28" s="45"/>
     </row>
@@ -9736,7 +9748,7 @@
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="47"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="44"/>
       <c r="F29" s="45"/>
     </row>
@@ -9746,7 +9758,7 @@
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="47"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="44"/>
       <c r="F30" s="45"/>
     </row>
@@ -9756,7 +9768,7 @@
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="47"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="44"/>
       <c r="F31" s="45"/>
     </row>
@@ -9766,7 +9778,7 @@
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="47"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="44"/>
       <c r="F32" s="45"/>
     </row>
@@ -9776,7 +9788,7 @@
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="47"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="44"/>
       <c r="F33" s="45"/>
     </row>
@@ -9786,7 +9798,7 @@
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="47"/>
+      <c r="D34" s="48"/>
       <c r="E34" s="44"/>
       <c r="F34" s="45"/>
     </row>
@@ -9796,7 +9808,7 @@
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="47"/>
+      <c r="D35" s="48"/>
       <c r="E35" s="44"/>
       <c r="F35" s="45"/>
     </row>
@@ -9806,7 +9818,7 @@
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="47"/>
+      <c r="D36" s="48"/>
       <c r="E36" s="44"/>
       <c r="F36" s="45"/>
     </row>
@@ -9816,7 +9828,7 @@
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="47"/>
+      <c r="D37" s="48"/>
       <c r="E37" s="44"/>
       <c r="F37" s="45"/>
     </row>
@@ -9826,7 +9838,7 @@
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="44"/>
       <c r="F38" s="45"/>
     </row>
@@ -9836,7 +9848,7 @@
       </c>
       <c r="B39" s="42"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="44"/>
       <c r="F39" s="45"/>
     </row>
@@ -9846,7 +9858,7 @@
       </c>
       <c r="B40" s="42"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="44"/>
       <c r="F40" s="45"/>
     </row>
@@ -9856,7 +9868,7 @@
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="44"/>
       <c r="F41" s="45"/>
     </row>
@@ -9866,7 +9878,7 @@
       </c>
       <c r="B42" s="42"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="47"/>
+      <c r="D42" s="48"/>
       <c r="E42" s="44"/>
       <c r="F42" s="45"/>
     </row>
@@ -9876,7 +9888,7 @@
       </c>
       <c r="B43" s="42"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="47"/>
+      <c r="D43" s="48"/>
       <c r="E43" s="44"/>
       <c r="F43" s="45"/>
     </row>
@@ -9886,7 +9898,7 @@
       </c>
       <c r="B44" s="42"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="47"/>
+      <c r="D44" s="48"/>
       <c r="E44" s="44"/>
       <c r="F44" s="45"/>
     </row>
@@ -9896,7 +9908,7 @@
       </c>
       <c r="B45" s="42"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="47"/>
+      <c r="D45" s="48"/>
       <c r="E45" s="44"/>
       <c r="F45" s="45"/>
     </row>
@@ -9906,7 +9918,7 @@
       </c>
       <c r="B46" s="42"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="47"/>
+      <c r="D46" s="48"/>
       <c r="E46" s="44"/>
       <c r="F46" s="45"/>
     </row>
@@ -9916,7 +9928,7 @@
       </c>
       <c r="B47" s="42"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="47"/>
+      <c r="D47" s="48"/>
       <c r="E47" s="44"/>
       <c r="F47" s="45"/>
     </row>
@@ -9926,7 +9938,7 @@
       </c>
       <c r="B48" s="42"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="47"/>
+      <c r="D48" s="48"/>
       <c r="E48" s="44"/>
       <c r="F48" s="45"/>
     </row>
@@ -9936,7 +9948,7 @@
       </c>
       <c r="B49" s="42"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="47"/>
+      <c r="D49" s="48"/>
       <c r="E49" s="44"/>
       <c r="F49" s="45"/>
     </row>
@@ -9946,7 +9958,7 @@
       </c>
       <c r="B50" s="42"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="47"/>
+      <c r="D50" s="48"/>
       <c r="E50" s="44"/>
       <c r="F50" s="45"/>
     </row>
@@ -9956,7 +9968,7 @@
       </c>
       <c r="B51" s="42"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="47"/>
+      <c r="D51" s="48"/>
       <c r="E51" s="44"/>
       <c r="F51" s="45"/>
     </row>
@@ -9966,7 +9978,7 @@
       </c>
       <c r="B52" s="42"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="47"/>
+      <c r="D52" s="48"/>
       <c r="E52" s="44"/>
       <c r="F52" s="45"/>
     </row>
@@ -9976,7 +9988,7 @@
       </c>
       <c r="B53" s="42"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="47"/>
+      <c r="D53" s="48"/>
       <c r="E53" s="44"/>
       <c r="F53" s="45"/>
     </row>
@@ -9986,7 +9998,7 @@
       </c>
       <c r="B54" s="42"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="47"/>
+      <c r="D54" s="48"/>
       <c r="E54" s="44"/>
       <c r="F54" s="45"/>
     </row>
@@ -9996,7 +10008,7 @@
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="47"/>
+      <c r="D55" s="48"/>
       <c r="E55" s="44"/>
       <c r="F55" s="45"/>
     </row>
@@ -10006,7 +10018,7 @@
       </c>
       <c r="B56" s="42"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="47"/>
+      <c r="D56" s="48"/>
       <c r="E56" s="44"/>
       <c r="F56" s="45"/>
     </row>
@@ -10016,7 +10028,7 @@
       </c>
       <c r="B57" s="42"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="47"/>
+      <c r="D57" s="48"/>
       <c r="E57" s="44"/>
       <c r="F57" s="45"/>
     </row>
@@ -10026,7 +10038,7 @@
       </c>
       <c r="B58" s="42"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="47"/>
+      <c r="D58" s="48"/>
       <c r="E58" s="44"/>
       <c r="F58" s="45"/>
     </row>
@@ -10036,7 +10048,7 @@
       </c>
       <c r="B59" s="42"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="47"/>
+      <c r="D59" s="48"/>
       <c r="E59" s="44"/>
       <c r="F59" s="45"/>
     </row>
@@ -10046,7 +10058,7 @@
       </c>
       <c r="B60" s="42"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="47"/>
+      <c r="D60" s="48"/>
       <c r="E60" s="44"/>
       <c r="F60" s="45"/>
     </row>
@@ -10056,7 +10068,7 @@
       </c>
       <c r="B61" s="42"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="47"/>
+      <c r="D61" s="48"/>
       <c r="E61" s="44"/>
       <c r="F61" s="45"/>
     </row>
@@ -10066,7 +10078,7 @@
       </c>
       <c r="B62" s="42"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="47"/>
+      <c r="D62" s="48"/>
       <c r="E62" s="44"/>
       <c r="F62" s="45"/>
     </row>
@@ -10076,7 +10088,7 @@
       </c>
       <c r="B63" s="42"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="47"/>
+      <c r="D63" s="48"/>
       <c r="E63" s="44"/>
       <c r="F63" s="45"/>
     </row>
@@ -10086,7 +10098,7 @@
       </c>
       <c r="B64" s="42"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="47"/>
+      <c r="D64" s="48"/>
       <c r="E64" s="44"/>
       <c r="F64" s="45"/>
     </row>
@@ -10096,7 +10108,7 @@
       </c>
       <c r="B65" s="42"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="47"/>
+      <c r="D65" s="48"/>
       <c r="E65" s="44"/>
       <c r="F65" s="45"/>
     </row>
@@ -10106,7 +10118,7 @@
       </c>
       <c r="B66" s="42"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="47"/>
+      <c r="D66" s="48"/>
       <c r="E66" s="44"/>
       <c r="F66" s="45"/>
     </row>
@@ -10116,7 +10128,7 @@
       </c>
       <c r="B67" s="42"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="47"/>
+      <c r="D67" s="48"/>
       <c r="E67" s="44"/>
       <c r="F67" s="45"/>
     </row>
@@ -10126,7 +10138,7 @@
       </c>
       <c r="B68" s="42"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="47"/>
+      <c r="D68" s="48"/>
       <c r="E68" s="44"/>
       <c r="F68" s="45"/>
     </row>
@@ -10136,7 +10148,7 @@
       </c>
       <c r="B69" s="42"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="47"/>
+      <c r="D69" s="48"/>
       <c r="E69" s="44"/>
       <c r="F69" s="45"/>
     </row>
@@ -10146,7 +10158,7 @@
       </c>
       <c r="B70" s="42"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="47"/>
+      <c r="D70" s="48"/>
       <c r="E70" s="44"/>
       <c r="F70" s="45"/>
     </row>
@@ -10156,7 +10168,7 @@
       </c>
       <c r="B71" s="42"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="47"/>
+      <c r="D71" s="48"/>
       <c r="E71" s="44"/>
       <c r="F71" s="45"/>
     </row>
@@ -10166,7 +10178,7 @@
       </c>
       <c r="B72" s="42"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="47"/>
+      <c r="D72" s="48"/>
       <c r="E72" s="44"/>
       <c r="F72" s="45"/>
     </row>
@@ -10176,7 +10188,7 @@
       </c>
       <c r="B73" s="42"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="47"/>
+      <c r="D73" s="48"/>
       <c r="E73" s="44"/>
       <c r="F73" s="45"/>
     </row>
@@ -10186,7 +10198,7 @@
       </c>
       <c r="B74" s="42"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="47"/>
+      <c r="D74" s="48"/>
       <c r="E74" s="44"/>
       <c r="F74" s="45"/>
     </row>
@@ -10196,7 +10208,7 @@
       </c>
       <c r="B75" s="42"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="47"/>
+      <c r="D75" s="48"/>
       <c r="E75" s="44"/>
       <c r="F75" s="45"/>
     </row>
@@ -10206,7 +10218,7 @@
       </c>
       <c r="B76" s="42"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="47"/>
+      <c r="D76" s="48"/>
       <c r="E76" s="44"/>
       <c r="F76" s="45"/>
     </row>
@@ -10216,7 +10228,7 @@
       </c>
       <c r="B77" s="42"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="47"/>
+      <c r="D77" s="48"/>
       <c r="E77" s="44"/>
       <c r="F77" s="45"/>
     </row>
@@ -10226,7 +10238,7 @@
       </c>
       <c r="B78" s="42"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="47"/>
+      <c r="D78" s="48"/>
       <c r="E78" s="44"/>
       <c r="F78" s="45"/>
     </row>
@@ -10236,7 +10248,7 @@
       </c>
       <c r="B79" s="42"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="47"/>
+      <c r="D79" s="48"/>
       <c r="E79" s="44"/>
       <c r="F79" s="45"/>
     </row>
@@ -10246,7 +10258,7 @@
       </c>
       <c r="B80" s="42"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="47"/>
+      <c r="D80" s="48"/>
       <c r="E80" s="44"/>
       <c r="F80" s="45"/>
     </row>
@@ -10256,7 +10268,7 @@
       </c>
       <c r="B81" s="42"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="47"/>
+      <c r="D81" s="48"/>
       <c r="E81" s="44"/>
       <c r="F81" s="45"/>
     </row>
@@ -10266,7 +10278,7 @@
       </c>
       <c r="B82" s="42"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="47"/>
+      <c r="D82" s="48"/>
       <c r="E82" s="44"/>
       <c r="F82" s="45"/>
     </row>
@@ -10276,7 +10288,7 @@
       </c>
       <c r="B83" s="42"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="47"/>
+      <c r="D83" s="48"/>
       <c r="E83" s="44"/>
       <c r="F83" s="45"/>
     </row>
@@ -10286,7 +10298,7 @@
       </c>
       <c r="B84" s="42"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="47"/>
+      <c r="D84" s="48"/>
       <c r="E84" s="44"/>
       <c r="F84" s="45"/>
     </row>
@@ -10296,7 +10308,7 @@
       </c>
       <c r="B85" s="42"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="47"/>
+      <c r="D85" s="48"/>
       <c r="E85" s="44"/>
       <c r="F85" s="45"/>
     </row>
@@ -10306,7 +10318,7 @@
       </c>
       <c r="B86" s="42"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="47"/>
+      <c r="D86" s="48"/>
       <c r="E86" s="44"/>
       <c r="F86" s="45"/>
     </row>
@@ -10316,7 +10328,7 @@
       </c>
       <c r="B87" s="42"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="47"/>
+      <c r="D87" s="48"/>
       <c r="E87" s="44"/>
       <c r="F87" s="45"/>
     </row>
@@ -10326,7 +10338,7 @@
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="47"/>
+      <c r="D88" s="48"/>
       <c r="E88" s="44"/>
       <c r="F88" s="45"/>
     </row>
@@ -10336,7 +10348,7 @@
       </c>
       <c r="B89" s="42"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="47"/>
+      <c r="D89" s="48"/>
       <c r="E89" s="44"/>
       <c r="F89" s="45"/>
     </row>
@@ -10346,7 +10358,7 @@
       </c>
       <c r="B90" s="42"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="47"/>
+      <c r="D90" s="48"/>
       <c r="E90" s="44"/>
       <c r="F90" s="45"/>
     </row>
@@ -10356,7 +10368,7 @@
       </c>
       <c r="B91" s="42"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="47"/>
+      <c r="D91" s="48"/>
       <c r="E91" s="44"/>
       <c r="F91" s="45"/>
     </row>
@@ -10366,7 +10378,7 @@
       </c>
       <c r="B92" s="42"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="47"/>
+      <c r="D92" s="48"/>
       <c r="E92" s="44"/>
       <c r="F92" s="45"/>
     </row>
@@ -10376,7 +10388,7 @@
       </c>
       <c r="B93" s="42"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="47"/>
+      <c r="D93" s="48"/>
       <c r="E93" s="44"/>
       <c r="F93" s="45"/>
     </row>
@@ -10386,7 +10398,7 @@
       </c>
       <c r="B94" s="42"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="47"/>
+      <c r="D94" s="48"/>
       <c r="E94" s="44"/>
       <c r="F94" s="45"/>
     </row>
@@ -10396,7 +10408,7 @@
       </c>
       <c r="B95" s="42"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="47"/>
+      <c r="D95" s="48"/>
       <c r="E95" s="44"/>
       <c r="F95" s="45"/>
     </row>
@@ -10406,7 +10418,7 @@
       </c>
       <c r="B96" s="42"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="47"/>
+      <c r="D96" s="48"/>
       <c r="E96" s="44"/>
       <c r="F96" s="45"/>
     </row>
@@ -10416,7 +10428,7 @@
       </c>
       <c r="B97" s="42"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="47"/>
+      <c r="D97" s="48"/>
       <c r="E97" s="44"/>
       <c r="F97" s="45"/>
     </row>
@@ -10426,7 +10438,7 @@
       </c>
       <c r="B98" s="42"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="47"/>
+      <c r="D98" s="48"/>
       <c r="E98" s="44"/>
       <c r="F98" s="45"/>
     </row>
@@ -10436,7 +10448,7 @@
       </c>
       <c r="B99" s="42"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="47"/>
+      <c r="D99" s="48"/>
       <c r="E99" s="44"/>
       <c r="F99" s="45"/>
     </row>
@@ -10446,7 +10458,7 @@
       </c>
       <c r="B100" s="42"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="47"/>
+      <c r="D100" s="48"/>
       <c r="E100" s="44"/>
       <c r="F100" s="45"/>
     </row>
@@ -10753,7 +10765,7 @@
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="47"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="44"/>
       <c r="F18" s="45"/>
     </row>
@@ -10763,7 +10775,7 @@
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="44"/>
       <c r="F19" s="45"/>
     </row>
@@ -10773,7 +10785,7 @@
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="44"/>
       <c r="F20" s="45"/>
     </row>
@@ -10783,7 +10795,7 @@
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="44"/>
       <c r="F21" s="45"/>
     </row>
@@ -10793,7 +10805,7 @@
       </c>
       <c r="B22" s="42"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="47"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="44"/>
       <c r="F22" s="45"/>
     </row>
@@ -10803,7 +10815,7 @@
       </c>
       <c r="B23" s="42"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="47"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="44"/>
       <c r="F23" s="45"/>
     </row>
@@ -10813,7 +10825,7 @@
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="47"/>
+      <c r="D24" s="48"/>
       <c r="E24" s="44"/>
       <c r="F24" s="45"/>
     </row>
@@ -10823,7 +10835,7 @@
       </c>
       <c r="B25" s="42"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="47"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="44"/>
       <c r="F25" s="45"/>
     </row>
@@ -10833,7 +10845,7 @@
       </c>
       <c r="B26" s="42"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="47"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="44"/>
       <c r="F26" s="45"/>
     </row>
@@ -10843,7 +10855,7 @@
       </c>
       <c r="B27" s="42"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="47"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="44"/>
       <c r="F27" s="45"/>
     </row>
@@ -10853,7 +10865,7 @@
       </c>
       <c r="B28" s="42"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="47"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="44"/>
       <c r="F28" s="45"/>
     </row>
@@ -10863,7 +10875,7 @@
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="47"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="44"/>
       <c r="F29" s="45"/>
     </row>
@@ -10873,7 +10885,7 @@
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="47"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="44"/>
       <c r="F30" s="45"/>
     </row>
@@ -10883,7 +10895,7 @@
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="47"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="44"/>
       <c r="F31" s="45"/>
     </row>
@@ -10893,7 +10905,7 @@
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="47"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="44"/>
       <c r="F32" s="45"/>
     </row>
@@ -10903,7 +10915,7 @@
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="47"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="44"/>
       <c r="F33" s="45"/>
     </row>
@@ -10913,7 +10925,7 @@
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="47"/>
+      <c r="D34" s="48"/>
       <c r="E34" s="44"/>
       <c r="F34" s="45"/>
     </row>
@@ -10923,7 +10935,7 @@
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="47"/>
+      <c r="D35" s="48"/>
       <c r="E35" s="44"/>
       <c r="F35" s="45"/>
     </row>
@@ -10933,7 +10945,7 @@
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="47"/>
+      <c r="D36" s="48"/>
       <c r="E36" s="44"/>
       <c r="F36" s="45"/>
     </row>
@@ -10943,7 +10955,7 @@
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="47"/>
+      <c r="D37" s="48"/>
       <c r="E37" s="44"/>
       <c r="F37" s="45"/>
     </row>
@@ -10953,7 +10965,7 @@
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="44"/>
       <c r="F38" s="45"/>
     </row>
@@ -10963,7 +10975,7 @@
       </c>
       <c r="B39" s="42"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="44"/>
       <c r="F39" s="45"/>
     </row>
@@ -10973,7 +10985,7 @@
       </c>
       <c r="B40" s="42"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="44"/>
       <c r="F40" s="45"/>
     </row>
@@ -10983,7 +10995,7 @@
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="44"/>
       <c r="F41" s="45"/>
     </row>
@@ -10993,7 +11005,7 @@
       </c>
       <c r="B42" s="42"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="47"/>
+      <c r="D42" s="48"/>
       <c r="E42" s="44"/>
       <c r="F42" s="45"/>
     </row>
@@ -11003,7 +11015,7 @@
       </c>
       <c r="B43" s="42"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="47"/>
+      <c r="D43" s="48"/>
       <c r="E43" s="44"/>
       <c r="F43" s="45"/>
     </row>
@@ -11013,7 +11025,7 @@
       </c>
       <c r="B44" s="42"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="47"/>
+      <c r="D44" s="48"/>
       <c r="E44" s="44"/>
       <c r="F44" s="45"/>
     </row>
@@ -11023,7 +11035,7 @@
       </c>
       <c r="B45" s="42"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="47"/>
+      <c r="D45" s="48"/>
       <c r="E45" s="44"/>
       <c r="F45" s="45"/>
     </row>
@@ -11033,7 +11045,7 @@
       </c>
       <c r="B46" s="42"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="47"/>
+      <c r="D46" s="48"/>
       <c r="E46" s="44"/>
       <c r="F46" s="45"/>
     </row>
@@ -11043,7 +11055,7 @@
       </c>
       <c r="B47" s="42"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="47"/>
+      <c r="D47" s="48"/>
       <c r="E47" s="44"/>
       <c r="F47" s="45"/>
     </row>
@@ -11053,7 +11065,7 @@
       </c>
       <c r="B48" s="42"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="47"/>
+      <c r="D48" s="48"/>
       <c r="E48" s="44"/>
       <c r="F48" s="45"/>
     </row>
@@ -11063,7 +11075,7 @@
       </c>
       <c r="B49" s="42"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="47"/>
+      <c r="D49" s="48"/>
       <c r="E49" s="44"/>
       <c r="F49" s="45"/>
     </row>
@@ -11073,7 +11085,7 @@
       </c>
       <c r="B50" s="42"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="47"/>
+      <c r="D50" s="48"/>
       <c r="E50" s="44"/>
       <c r="F50" s="45"/>
     </row>
@@ -11083,7 +11095,7 @@
       </c>
       <c r="B51" s="42"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="47"/>
+      <c r="D51" s="48"/>
       <c r="E51" s="44"/>
       <c r="F51" s="45"/>
     </row>
@@ -11093,7 +11105,7 @@
       </c>
       <c r="B52" s="42"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="47"/>
+      <c r="D52" s="48"/>
       <c r="E52" s="44"/>
       <c r="F52" s="45"/>
     </row>
@@ -11103,7 +11115,7 @@
       </c>
       <c r="B53" s="42"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="47"/>
+      <c r="D53" s="48"/>
       <c r="E53" s="44"/>
       <c r="F53" s="45"/>
     </row>
@@ -11113,7 +11125,7 @@
       </c>
       <c r="B54" s="42"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="47"/>
+      <c r="D54" s="48"/>
       <c r="E54" s="44"/>
       <c r="F54" s="45"/>
     </row>
@@ -11123,7 +11135,7 @@
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="47"/>
+      <c r="D55" s="48"/>
       <c r="E55" s="44"/>
       <c r="F55" s="45"/>
     </row>
@@ -11133,7 +11145,7 @@
       </c>
       <c r="B56" s="42"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="47"/>
+      <c r="D56" s="48"/>
       <c r="E56" s="44"/>
       <c r="F56" s="45"/>
     </row>
@@ -11143,7 +11155,7 @@
       </c>
       <c r="B57" s="42"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="47"/>
+      <c r="D57" s="48"/>
       <c r="E57" s="44"/>
       <c r="F57" s="45"/>
     </row>
@@ -11153,7 +11165,7 @@
       </c>
       <c r="B58" s="42"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="47"/>
+      <c r="D58" s="48"/>
       <c r="E58" s="44"/>
       <c r="F58" s="45"/>
     </row>
@@ -11163,7 +11175,7 @@
       </c>
       <c r="B59" s="42"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="47"/>
+      <c r="D59" s="48"/>
       <c r="E59" s="44"/>
       <c r="F59" s="45"/>
     </row>
@@ -11173,7 +11185,7 @@
       </c>
       <c r="B60" s="42"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="47"/>
+      <c r="D60" s="48"/>
       <c r="E60" s="44"/>
       <c r="F60" s="45"/>
     </row>
@@ -11183,7 +11195,7 @@
       </c>
       <c r="B61" s="42"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="47"/>
+      <c r="D61" s="48"/>
       <c r="E61" s="44"/>
       <c r="F61" s="45"/>
     </row>
@@ -11193,7 +11205,7 @@
       </c>
       <c r="B62" s="42"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="47"/>
+      <c r="D62" s="48"/>
       <c r="E62" s="44"/>
       <c r="F62" s="45"/>
     </row>
@@ -11203,7 +11215,7 @@
       </c>
       <c r="B63" s="42"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="47"/>
+      <c r="D63" s="48"/>
       <c r="E63" s="44"/>
       <c r="F63" s="45"/>
     </row>
@@ -11213,7 +11225,7 @@
       </c>
       <c r="B64" s="42"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="47"/>
+      <c r="D64" s="48"/>
       <c r="E64" s="44"/>
       <c r="F64" s="45"/>
     </row>
@@ -11223,7 +11235,7 @@
       </c>
       <c r="B65" s="42"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="47"/>
+      <c r="D65" s="48"/>
       <c r="E65" s="44"/>
       <c r="F65" s="45"/>
     </row>
@@ -11233,7 +11245,7 @@
       </c>
       <c r="B66" s="42"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="47"/>
+      <c r="D66" s="48"/>
       <c r="E66" s="44"/>
       <c r="F66" s="45"/>
     </row>
@@ -11243,7 +11255,7 @@
       </c>
       <c r="B67" s="42"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="47"/>
+      <c r="D67" s="48"/>
       <c r="E67" s="44"/>
       <c r="F67" s="45"/>
     </row>
@@ -11253,7 +11265,7 @@
       </c>
       <c r="B68" s="42"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="47"/>
+      <c r="D68" s="48"/>
       <c r="E68" s="44"/>
       <c r="F68" s="45"/>
     </row>
@@ -11263,7 +11275,7 @@
       </c>
       <c r="B69" s="42"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="47"/>
+      <c r="D69" s="48"/>
       <c r="E69" s="44"/>
       <c r="F69" s="45"/>
     </row>
@@ -11273,7 +11285,7 @@
       </c>
       <c r="B70" s="42"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="47"/>
+      <c r="D70" s="48"/>
       <c r="E70" s="44"/>
       <c r="F70" s="45"/>
     </row>
@@ -11283,7 +11295,7 @@
       </c>
       <c r="B71" s="42"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="47"/>
+      <c r="D71" s="48"/>
       <c r="E71" s="44"/>
       <c r="F71" s="45"/>
     </row>
@@ -11293,7 +11305,7 @@
       </c>
       <c r="B72" s="42"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="47"/>
+      <c r="D72" s="48"/>
       <c r="E72" s="44"/>
       <c r="F72" s="45"/>
     </row>
@@ -11303,7 +11315,7 @@
       </c>
       <c r="B73" s="42"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="47"/>
+      <c r="D73" s="48"/>
       <c r="E73" s="44"/>
       <c r="F73" s="45"/>
     </row>
@@ -11313,7 +11325,7 @@
       </c>
       <c r="B74" s="42"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="47"/>
+      <c r="D74" s="48"/>
       <c r="E74" s="44"/>
       <c r="F74" s="45"/>
     </row>
@@ -11323,7 +11335,7 @@
       </c>
       <c r="B75" s="42"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="47"/>
+      <c r="D75" s="48"/>
       <c r="E75" s="44"/>
       <c r="F75" s="45"/>
     </row>
@@ -11333,7 +11345,7 @@
       </c>
       <c r="B76" s="42"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="47"/>
+      <c r="D76" s="48"/>
       <c r="E76" s="44"/>
       <c r="F76" s="45"/>
     </row>
@@ -11343,7 +11355,7 @@
       </c>
       <c r="B77" s="42"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="47"/>
+      <c r="D77" s="48"/>
       <c r="E77" s="44"/>
       <c r="F77" s="45"/>
     </row>
@@ -11353,7 +11365,7 @@
       </c>
       <c r="B78" s="42"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="47"/>
+      <c r="D78" s="48"/>
       <c r="E78" s="44"/>
       <c r="F78" s="45"/>
     </row>
@@ -11363,7 +11375,7 @@
       </c>
       <c r="B79" s="42"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="47"/>
+      <c r="D79" s="48"/>
       <c r="E79" s="44"/>
       <c r="F79" s="45"/>
     </row>
@@ -11373,7 +11385,7 @@
       </c>
       <c r="B80" s="42"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="47"/>
+      <c r="D80" s="48"/>
       <c r="E80" s="44"/>
       <c r="F80" s="45"/>
     </row>
@@ -11383,7 +11395,7 @@
       </c>
       <c r="B81" s="42"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="47"/>
+      <c r="D81" s="48"/>
       <c r="E81" s="44"/>
       <c r="F81" s="45"/>
     </row>
@@ -11393,7 +11405,7 @@
       </c>
       <c r="B82" s="42"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="47"/>
+      <c r="D82" s="48"/>
       <c r="E82" s="44"/>
       <c r="F82" s="45"/>
     </row>
@@ -11403,7 +11415,7 @@
       </c>
       <c r="B83" s="42"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="47"/>
+      <c r="D83" s="48"/>
       <c r="E83" s="44"/>
       <c r="F83" s="45"/>
     </row>
@@ -11413,7 +11425,7 @@
       </c>
       <c r="B84" s="42"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="47"/>
+      <c r="D84" s="48"/>
       <c r="E84" s="44"/>
       <c r="F84" s="45"/>
     </row>
@@ -11423,7 +11435,7 @@
       </c>
       <c r="B85" s="42"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="47"/>
+      <c r="D85" s="48"/>
       <c r="E85" s="44"/>
       <c r="F85" s="45"/>
     </row>
@@ -11433,7 +11445,7 @@
       </c>
       <c r="B86" s="42"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="47"/>
+      <c r="D86" s="48"/>
       <c r="E86" s="44"/>
       <c r="F86" s="45"/>
     </row>
@@ -11443,7 +11455,7 @@
       </c>
       <c r="B87" s="42"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="47"/>
+      <c r="D87" s="48"/>
       <c r="E87" s="44"/>
       <c r="F87" s="45"/>
     </row>
@@ -11453,7 +11465,7 @@
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="47"/>
+      <c r="D88" s="48"/>
       <c r="E88" s="44"/>
       <c r="F88" s="45"/>
     </row>
@@ -11463,7 +11475,7 @@
       </c>
       <c r="B89" s="42"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="47"/>
+      <c r="D89" s="48"/>
       <c r="E89" s="44"/>
       <c r="F89" s="45"/>
     </row>
@@ -11473,7 +11485,7 @@
       </c>
       <c r="B90" s="42"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="47"/>
+      <c r="D90" s="48"/>
       <c r="E90" s="44"/>
       <c r="F90" s="45"/>
     </row>
@@ -11483,7 +11495,7 @@
       </c>
       <c r="B91" s="42"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="47"/>
+      <c r="D91" s="48"/>
       <c r="E91" s="44"/>
       <c r="F91" s="45"/>
     </row>
@@ -11493,7 +11505,7 @@
       </c>
       <c r="B92" s="42"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="47"/>
+      <c r="D92" s="48"/>
       <c r="E92" s="44"/>
       <c r="F92" s="45"/>
     </row>
@@ -11503,7 +11515,7 @@
       </c>
       <c r="B93" s="42"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="47"/>
+      <c r="D93" s="48"/>
       <c r="E93" s="44"/>
       <c r="F93" s="45"/>
     </row>
@@ -11513,7 +11525,7 @@
       </c>
       <c r="B94" s="42"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="47"/>
+      <c r="D94" s="48"/>
       <c r="E94" s="44"/>
       <c r="F94" s="45"/>
     </row>
@@ -11523,7 +11535,7 @@
       </c>
       <c r="B95" s="42"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="47"/>
+      <c r="D95" s="48"/>
       <c r="E95" s="44"/>
       <c r="F95" s="45"/>
     </row>
@@ -11533,7 +11545,7 @@
       </c>
       <c r="B96" s="42"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="47"/>
+      <c r="D96" s="48"/>
       <c r="E96" s="44"/>
       <c r="F96" s="45"/>
     </row>
@@ -11543,7 +11555,7 @@
       </c>
       <c r="B97" s="42"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="47"/>
+      <c r="D97" s="48"/>
       <c r="E97" s="44"/>
       <c r="F97" s="45"/>
     </row>
@@ -11553,7 +11565,7 @@
       </c>
       <c r="B98" s="42"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="47"/>
+      <c r="D98" s="48"/>
       <c r="E98" s="44"/>
       <c r="F98" s="45"/>
     </row>
@@ -11563,7 +11575,7 @@
       </c>
       <c r="B99" s="42"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="47"/>
+      <c r="D99" s="48"/>
       <c r="E99" s="44"/>
       <c r="F99" s="45"/>
     </row>
@@ -11573,7 +11585,7 @@
       </c>
       <c r="B100" s="42"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="47"/>
+      <c r="D100" s="48"/>
       <c r="E100" s="44"/>
       <c r="F100" s="45"/>
     </row>
@@ -11643,7 +11655,7 @@
         <f aca="false">'Sprint 05 Backlog'!B1+1</f>
         <v>6</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="49" t="s">
         <v>204</v>
       </c>
       <c r="D1" s="33" t="s">
@@ -11840,7 +11852,7 @@
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="49" t="s">
         <v>205</v>
       </c>
       <c r="E15" s="32"/>
@@ -11884,7 +11896,7 @@
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="47"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="44"/>
       <c r="F18" s="45"/>
     </row>
@@ -11894,7 +11906,7 @@
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="44"/>
       <c r="F19" s="45"/>
     </row>
@@ -11904,7 +11916,7 @@
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="44"/>
       <c r="F20" s="45"/>
     </row>
@@ -11914,7 +11926,7 @@
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="44"/>
       <c r="F21" s="45"/>
     </row>
@@ -11924,7 +11936,7 @@
       </c>
       <c r="B22" s="42"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="47"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="44"/>
       <c r="F22" s="45"/>
     </row>
@@ -11934,7 +11946,7 @@
       </c>
       <c r="B23" s="42"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="47"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="44"/>
       <c r="F23" s="45"/>
     </row>
@@ -11944,7 +11956,7 @@
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="47"/>
+      <c r="D24" s="48"/>
       <c r="E24" s="44"/>
       <c r="F24" s="45"/>
     </row>
@@ -11954,7 +11966,7 @@
       </c>
       <c r="B25" s="42"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="47"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="44"/>
       <c r="F25" s="45"/>
     </row>
@@ -11964,7 +11976,7 @@
       </c>
       <c r="B26" s="42"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="47"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="44"/>
       <c r="F26" s="45"/>
     </row>
@@ -11974,7 +11986,7 @@
       </c>
       <c r="B27" s="42"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="47"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="44"/>
       <c r="F27" s="45"/>
     </row>
@@ -11984,7 +11996,7 @@
       </c>
       <c r="B28" s="42"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="47"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="44"/>
       <c r="F28" s="45"/>
     </row>
@@ -11994,7 +12006,7 @@
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="47"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="44"/>
       <c r="F29" s="45"/>
     </row>
@@ -12004,7 +12016,7 @@
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="47"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="44"/>
       <c r="F30" s="45"/>
     </row>
@@ -12014,7 +12026,7 @@
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="47"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="44"/>
       <c r="F31" s="45"/>
     </row>
@@ -12024,7 +12036,7 @@
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="47"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="44"/>
       <c r="F32" s="45"/>
     </row>
@@ -12034,7 +12046,7 @@
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="47"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="44"/>
       <c r="F33" s="45"/>
     </row>
@@ -12044,7 +12056,7 @@
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="47"/>
+      <c r="D34" s="48"/>
       <c r="E34" s="44"/>
       <c r="F34" s="45"/>
     </row>
@@ -12054,7 +12066,7 @@
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="47"/>
+      <c r="D35" s="48"/>
       <c r="E35" s="44"/>
       <c r="F35" s="45"/>
     </row>
@@ -12064,7 +12076,7 @@
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="47"/>
+      <c r="D36" s="48"/>
       <c r="E36" s="44"/>
       <c r="F36" s="45"/>
     </row>
@@ -12074,7 +12086,7 @@
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="47"/>
+      <c r="D37" s="48"/>
       <c r="E37" s="44"/>
       <c r="F37" s="45"/>
     </row>
@@ -12084,7 +12096,7 @@
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="44"/>
       <c r="F38" s="45"/>
     </row>
@@ -12094,7 +12106,7 @@
       </c>
       <c r="B39" s="42"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="44"/>
       <c r="F39" s="45"/>
     </row>
@@ -12104,7 +12116,7 @@
       </c>
       <c r="B40" s="42"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="44"/>
       <c r="F40" s="45"/>
     </row>
@@ -12114,7 +12126,7 @@
       </c>
       <c r="B41" s="42"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="44"/>
       <c r="F41" s="45"/>
     </row>
@@ -12124,7 +12136,7 @@
       </c>
       <c r="B42" s="42"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="47"/>
+      <c r="D42" s="48"/>
       <c r="E42" s="44"/>
       <c r="F42" s="45"/>
     </row>
@@ -12134,7 +12146,7 @@
       </c>
       <c r="B43" s="42"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="47"/>
+      <c r="D43" s="48"/>
       <c r="E43" s="44"/>
       <c r="F43" s="45"/>
     </row>
@@ -12144,7 +12156,7 @@
       </c>
       <c r="B44" s="42"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="47"/>
+      <c r="D44" s="48"/>
       <c r="E44" s="44"/>
       <c r="F44" s="45"/>
     </row>
@@ -12154,7 +12166,7 @@
       </c>
       <c r="B45" s="42"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="47"/>
+      <c r="D45" s="48"/>
       <c r="E45" s="44"/>
       <c r="F45" s="45"/>
     </row>
@@ -12164,7 +12176,7 @@
       </c>
       <c r="B46" s="42"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="47"/>
+      <c r="D46" s="48"/>
       <c r="E46" s="44"/>
       <c r="F46" s="45"/>
     </row>
@@ -12174,7 +12186,7 @@
       </c>
       <c r="B47" s="42"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="47"/>
+      <c r="D47" s="48"/>
       <c r="E47" s="44"/>
       <c r="F47" s="45"/>
     </row>
@@ -12184,7 +12196,7 @@
       </c>
       <c r="B48" s="42"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="47"/>
+      <c r="D48" s="48"/>
       <c r="E48" s="44"/>
       <c r="F48" s="45"/>
     </row>
@@ -12194,7 +12206,7 @@
       </c>
       <c r="B49" s="42"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="47"/>
+      <c r="D49" s="48"/>
       <c r="E49" s="44"/>
       <c r="F49" s="45"/>
     </row>
@@ -12204,7 +12216,7 @@
       </c>
       <c r="B50" s="42"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="47"/>
+      <c r="D50" s="48"/>
       <c r="E50" s="44"/>
       <c r="F50" s="45"/>
     </row>
@@ -12214,7 +12226,7 @@
       </c>
       <c r="B51" s="42"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="47"/>
+      <c r="D51" s="48"/>
       <c r="E51" s="44"/>
       <c r="F51" s="45"/>
     </row>
@@ -12224,7 +12236,7 @@
       </c>
       <c r="B52" s="42"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="47"/>
+      <c r="D52" s="48"/>
       <c r="E52" s="44"/>
       <c r="F52" s="45"/>
     </row>
@@ -12234,7 +12246,7 @@
       </c>
       <c r="B53" s="42"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="47"/>
+      <c r="D53" s="48"/>
       <c r="E53" s="44"/>
       <c r="F53" s="45"/>
     </row>
@@ -12244,7 +12256,7 @@
       </c>
       <c r="B54" s="42"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="47"/>
+      <c r="D54" s="48"/>
       <c r="E54" s="44"/>
       <c r="F54" s="45"/>
     </row>
@@ -12254,7 +12266,7 @@
       </c>
       <c r="B55" s="42"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="47"/>
+      <c r="D55" s="48"/>
       <c r="E55" s="44"/>
       <c r="F55" s="45"/>
     </row>
@@ -12264,7 +12276,7 @@
       </c>
       <c r="B56" s="42"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="47"/>
+      <c r="D56" s="48"/>
       <c r="E56" s="44"/>
       <c r="F56" s="45"/>
     </row>
@@ -12274,7 +12286,7 @@
       </c>
       <c r="B57" s="42"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="47"/>
+      <c r="D57" s="48"/>
       <c r="E57" s="44"/>
       <c r="F57" s="45"/>
     </row>
@@ -12284,7 +12296,7 @@
       </c>
       <c r="B58" s="42"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="47"/>
+      <c r="D58" s="48"/>
       <c r="E58" s="44"/>
       <c r="F58" s="45"/>
     </row>
@@ -12294,7 +12306,7 @@
       </c>
       <c r="B59" s="42"/>
       <c r="C59" s="1"/>
-      <c r="D59" s="47"/>
+      <c r="D59" s="48"/>
       <c r="E59" s="44"/>
       <c r="F59" s="45"/>
     </row>
@@ -12304,7 +12316,7 @@
       </c>
       <c r="B60" s="42"/>
       <c r="C60" s="1"/>
-      <c r="D60" s="47"/>
+      <c r="D60" s="48"/>
       <c r="E60" s="44"/>
       <c r="F60" s="45"/>
     </row>
@@ -12314,7 +12326,7 @@
       </c>
       <c r="B61" s="42"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="47"/>
+      <c r="D61" s="48"/>
       <c r="E61" s="44"/>
       <c r="F61" s="45"/>
     </row>
@@ -12324,7 +12336,7 @@
       </c>
       <c r="B62" s="42"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="47"/>
+      <c r="D62" s="48"/>
       <c r="E62" s="44"/>
       <c r="F62" s="45"/>
     </row>
@@ -12334,7 +12346,7 @@
       </c>
       <c r="B63" s="42"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="47"/>
+      <c r="D63" s="48"/>
       <c r="E63" s="44"/>
       <c r="F63" s="45"/>
     </row>
@@ -12344,7 +12356,7 @@
       </c>
       <c r="B64" s="42"/>
       <c r="C64" s="1"/>
-      <c r="D64" s="47"/>
+      <c r="D64" s="48"/>
       <c r="E64" s="44"/>
       <c r="F64" s="45"/>
     </row>
@@ -12354,7 +12366,7 @@
       </c>
       <c r="B65" s="42"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="47"/>
+      <c r="D65" s="48"/>
       <c r="E65" s="44"/>
       <c r="F65" s="45"/>
     </row>
@@ -12364,7 +12376,7 @@
       </c>
       <c r="B66" s="42"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="47"/>
+      <c r="D66" s="48"/>
       <c r="E66" s="44"/>
       <c r="F66" s="45"/>
     </row>
@@ -12374,7 +12386,7 @@
       </c>
       <c r="B67" s="42"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="47"/>
+      <c r="D67" s="48"/>
       <c r="E67" s="44"/>
       <c r="F67" s="45"/>
     </row>
@@ -12384,7 +12396,7 @@
       </c>
       <c r="B68" s="42"/>
       <c r="C68" s="1"/>
-      <c r="D68" s="47"/>
+      <c r="D68" s="48"/>
       <c r="E68" s="44"/>
       <c r="F68" s="45"/>
     </row>
@@ -12394,7 +12406,7 @@
       </c>
       <c r="B69" s="42"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="47"/>
+      <c r="D69" s="48"/>
       <c r="E69" s="44"/>
       <c r="F69" s="45"/>
     </row>
@@ -12404,7 +12416,7 @@
       </c>
       <c r="B70" s="42"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="47"/>
+      <c r="D70" s="48"/>
       <c r="E70" s="44"/>
       <c r="F70" s="45"/>
     </row>
@@ -12414,7 +12426,7 @@
       </c>
       <c r="B71" s="42"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="47"/>
+      <c r="D71" s="48"/>
       <c r="E71" s="44"/>
       <c r="F71" s="45"/>
     </row>
@@ -12424,7 +12436,7 @@
       </c>
       <c r="B72" s="42"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="47"/>
+      <c r="D72" s="48"/>
       <c r="E72" s="44"/>
       <c r="F72" s="45"/>
     </row>
@@ -12434,7 +12446,7 @@
       </c>
       <c r="B73" s="42"/>
       <c r="C73" s="1"/>
-      <c r="D73" s="47"/>
+      <c r="D73" s="48"/>
       <c r="E73" s="44"/>
       <c r="F73" s="45"/>
     </row>
@@ -12444,7 +12456,7 @@
       </c>
       <c r="B74" s="42"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="47"/>
+      <c r="D74" s="48"/>
       <c r="E74" s="44"/>
       <c r="F74" s="45"/>
     </row>
@@ -12454,7 +12466,7 @@
       </c>
       <c r="B75" s="42"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="47"/>
+      <c r="D75" s="48"/>
       <c r="E75" s="44"/>
       <c r="F75" s="45"/>
     </row>
@@ -12464,7 +12476,7 @@
       </c>
       <c r="B76" s="42"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="47"/>
+      <c r="D76" s="48"/>
       <c r="E76" s="44"/>
       <c r="F76" s="45"/>
     </row>
@@ -12474,7 +12486,7 @@
       </c>
       <c r="B77" s="42"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="47"/>
+      <c r="D77" s="48"/>
       <c r="E77" s="44"/>
       <c r="F77" s="45"/>
     </row>
@@ -12484,7 +12496,7 @@
       </c>
       <c r="B78" s="42"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="47"/>
+      <c r="D78" s="48"/>
       <c r="E78" s="44"/>
       <c r="F78" s="45"/>
     </row>
@@ -12494,7 +12506,7 @@
       </c>
       <c r="B79" s="42"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="47"/>
+      <c r="D79" s="48"/>
       <c r="E79" s="44"/>
       <c r="F79" s="45"/>
     </row>
@@ -12504,7 +12516,7 @@
       </c>
       <c r="B80" s="42"/>
       <c r="C80" s="1"/>
-      <c r="D80" s="47"/>
+      <c r="D80" s="48"/>
       <c r="E80" s="44"/>
       <c r="F80" s="45"/>
     </row>
@@ -12514,7 +12526,7 @@
       </c>
       <c r="B81" s="42"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="47"/>
+      <c r="D81" s="48"/>
       <c r="E81" s="44"/>
       <c r="F81" s="45"/>
     </row>
@@ -12524,7 +12536,7 @@
       </c>
       <c r="B82" s="42"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="47"/>
+      <c r="D82" s="48"/>
       <c r="E82" s="44"/>
       <c r="F82" s="45"/>
     </row>
@@ -12534,7 +12546,7 @@
       </c>
       <c r="B83" s="42"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="47"/>
+      <c r="D83" s="48"/>
       <c r="E83" s="44"/>
       <c r="F83" s="45"/>
     </row>
@@ -12544,7 +12556,7 @@
       </c>
       <c r="B84" s="42"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="47"/>
+      <c r="D84" s="48"/>
       <c r="E84" s="44"/>
       <c r="F84" s="45"/>
     </row>
@@ -12554,7 +12566,7 @@
       </c>
       <c r="B85" s="42"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="47"/>
+      <c r="D85" s="48"/>
       <c r="E85" s="44"/>
       <c r="F85" s="45"/>
     </row>
@@ -12564,7 +12576,7 @@
       </c>
       <c r="B86" s="42"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="47"/>
+      <c r="D86" s="48"/>
       <c r="E86" s="44"/>
       <c r="F86" s="45"/>
     </row>
@@ -12574,7 +12586,7 @@
       </c>
       <c r="B87" s="42"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="47"/>
+      <c r="D87" s="48"/>
       <c r="E87" s="44"/>
       <c r="F87" s="45"/>
     </row>
@@ -12584,7 +12596,7 @@
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="47"/>
+      <c r="D88" s="48"/>
       <c r="E88" s="44"/>
       <c r="F88" s="45"/>
     </row>
@@ -12594,7 +12606,7 @@
       </c>
       <c r="B89" s="42"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="47"/>
+      <c r="D89" s="48"/>
       <c r="E89" s="44"/>
       <c r="F89" s="45"/>
     </row>
@@ -12604,7 +12616,7 @@
       </c>
       <c r="B90" s="42"/>
       <c r="C90" s="1"/>
-      <c r="D90" s="47"/>
+      <c r="D90" s="48"/>
       <c r="E90" s="44"/>
       <c r="F90" s="45"/>
     </row>
@@ -12614,7 +12626,7 @@
       </c>
       <c r="B91" s="42"/>
       <c r="C91" s="1"/>
-      <c r="D91" s="47"/>
+      <c r="D91" s="48"/>
       <c r="E91" s="44"/>
       <c r="F91" s="45"/>
     </row>
@@ -12624,7 +12636,7 @@
       </c>
       <c r="B92" s="42"/>
       <c r="C92" s="1"/>
-      <c r="D92" s="47"/>
+      <c r="D92" s="48"/>
       <c r="E92" s="44"/>
       <c r="F92" s="45"/>
     </row>
@@ -12634,7 +12646,7 @@
       </c>
       <c r="B93" s="42"/>
       <c r="C93" s="1"/>
-      <c r="D93" s="47"/>
+      <c r="D93" s="48"/>
       <c r="E93" s="44"/>
       <c r="F93" s="45"/>
     </row>
@@ -12644,7 +12656,7 @@
       </c>
       <c r="B94" s="42"/>
       <c r="C94" s="1"/>
-      <c r="D94" s="47"/>
+      <c r="D94" s="48"/>
       <c r="E94" s="44"/>
       <c r="F94" s="45"/>
     </row>
@@ -12654,7 +12666,7 @@
       </c>
       <c r="B95" s="42"/>
       <c r="C95" s="1"/>
-      <c r="D95" s="47"/>
+      <c r="D95" s="48"/>
       <c r="E95" s="44"/>
       <c r="F95" s="45"/>
     </row>
@@ -12664,7 +12676,7 @@
       </c>
       <c r="B96" s="42"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="47"/>
+      <c r="D96" s="48"/>
       <c r="E96" s="44"/>
       <c r="F96" s="45"/>
     </row>
@@ -12674,7 +12686,7 @@
       </c>
       <c r="B97" s="42"/>
       <c r="C97" s="1"/>
-      <c r="D97" s="47"/>
+      <c r="D97" s="48"/>
       <c r="E97" s="44"/>
       <c r="F97" s="45"/>
     </row>
@@ -12684,7 +12696,7 @@
       </c>
       <c r="B98" s="42"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="47"/>
+      <c r="D98" s="48"/>
       <c r="E98" s="44"/>
       <c r="F98" s="45"/>
     </row>
@@ -12694,7 +12706,7 @@
       </c>
       <c r="B99" s="42"/>
       <c r="C99" s="1"/>
-      <c r="D99" s="47"/>
+      <c r="D99" s="48"/>
       <c r="E99" s="44"/>
       <c r="F99" s="45"/>
     </row>
@@ -12704,7 +12716,7 @@
       </c>
       <c r="B100" s="42"/>
       <c r="C100" s="1"/>
-      <c r="D100" s="47"/>
+      <c r="D100" s="48"/>
       <c r="E100" s="44"/>
       <c r="F100" s="45"/>
     </row>

</xml_diff>

<commit_message>
P07 Create Graphics 3/20/2023 10:12 PM
</commit_message>
<xml_diff>
--- a/P07/Scrum_Sprint_3.xlsx
+++ b/P07/Scrum_Sprint_3.xlsx
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="208">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -705,6 +705,9 @@
   </si>
   <si>
     <t xml:space="preserve">Add to GitHub - Create a new, empty store </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write – Design Graph</t>
   </si>
   <si>
     <t xml:space="preserve">BONUS</t>
@@ -1215,1552 +1218,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 02 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="20144321"/>
-        <c:axId val="12843430"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="20144321"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="12843430"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="12843430"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="6480">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="20144321"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 03 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="61703437"/>
-        <c:axId val="18845699"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="61703437"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="18845699"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="18845699"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="6480">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="61703437"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 04 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="23304726"/>
-        <c:axId val="5706520"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="23304726"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="5706520"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="5706520"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="6480">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="23304726"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 05 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="45812547"/>
-        <c:axId val="74615322"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="45812547"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="74615322"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="74615322"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="6480">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="45812547"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 06 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="53725713"/>
-        <c:axId val="18227149"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="53725713"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="18227149"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="18227149"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="6480">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="53725713"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2912,11 +1370,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="74193151"/>
-        <c:axId val="36616078"/>
+        <c:axId val="48167529"/>
+        <c:axId val="7204921"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74193151"/>
+        <c:axId val="48167529"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -2984,12 +1442,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36616078"/>
+        <c:crossAx val="7204921"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="36616078"/>
+        <c:axId val="7204921"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3066,7 +1524,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74193151"/>
+        <c:crossAx val="48167529"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3093,7 +1551,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3221,11 +1679,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="38989248"/>
-        <c:axId val="37722246"/>
+        <c:axId val="26336050"/>
+        <c:axId val="99613795"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="38989248"/>
+        <c:axId val="26336050"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3291,7 +1749,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37722246"/>
+        <c:crossAx val="99613795"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3299,7 +1757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37722246"/>
+        <c:axId val="99613795"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3375,7 +1833,1552 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38989248"/>
+        <c:crossAx val="26336050"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 02 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="2098009"/>
+        <c:axId val="83938724"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2098009"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="83938724"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="83938724"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="6480">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2098009"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 03 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="8843455"/>
+        <c:axId val="65651500"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="8843455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65651500"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="65651500"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="6480">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="8843455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 04 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="92736001"/>
+        <c:axId val="73664156"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="92736001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="73664156"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="73664156"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="6480">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="92736001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 05 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="92640251"/>
+        <c:axId val="43462939"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="92640251"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="43462939"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43462939"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="6480">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="92640251"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 06 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="70085744"/>
+        <c:axId val="21387531"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="70085744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="21387531"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="21387531"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="6480">
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="70085744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3655,8 +3658,8 @@
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I34" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I38" activeCellId="0" sqref="I38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8059,8 +8062,8 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8152,7 +8155,7 @@
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -8165,7 +8168,7 @@
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">B7-C8</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -8181,7 +8184,7 @@
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">B8-C9</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -8197,7 +8200,7 @@
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">B9-C10</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -8213,7 +8216,7 @@
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">B10-C11</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -8229,7 +8232,7 @@
       </c>
       <c r="B12" s="32" t="n">
         <f aca="false">B11-C12</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -8245,7 +8248,7 @@
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">B12-C13</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -8261,7 +8264,7 @@
       </c>
       <c r="B14" s="32" t="n">
         <f aca="false">B13-C14</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -8585,15 +8588,23 @@
         <v>161</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B34" s="42"/>
+      <c r="B34" s="42" t="s">
+        <v>80</v>
+      </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="45"/>
+      <c r="D34" s="46" t="s">
+        <v>205</v>
+      </c>
+      <c r="E34" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" s="45" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -11580,7 +11591,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>2</v>
@@ -11777,7 +11788,7 @@
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="50" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>

</xml_diff>

<commit_message>
P07 Last Item - Create Graphics 3/21/2023 12:57 AM
</commit_message>
<xml_diff>
--- a/P07/Scrum_Sprint_3.xlsx
+++ b/P07/Scrum_Sprint_3.xlsx
@@ -82,6 +82,20 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">git commit -m "P07 Create a new, empty store 3/20/2023 3:15 PM"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">git commit -m "P07 Create Graphics 3/20/2023 10:12 PM"
+</t>
         </r>
       </text>
     </comment>
@@ -1218,7 +1232,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1370,11 +1384,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="48167529"/>
-        <c:axId val="7204921"/>
+        <c:axId val="79115450"/>
+        <c:axId val="21830319"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48167529"/>
+        <c:axId val="79115450"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1442,12 +1456,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7204921"/>
+        <c:crossAx val="21830319"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="7204921"/>
+        <c:axId val="21830319"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1524,7 +1538,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48167529"/>
+        <c:crossAx val="79115450"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1551,7 +1565,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1679,11 +1693,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="26336050"/>
-        <c:axId val="99613795"/>
+        <c:axId val="15432580"/>
+        <c:axId val="35846606"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="26336050"/>
+        <c:axId val="15432580"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1749,7 +1763,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99613795"/>
+        <c:crossAx val="35846606"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1757,7 +1771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99613795"/>
+        <c:axId val="35846606"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1833,7 +1847,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26336050"/>
+        <c:crossAx val="15432580"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1860,7 +1874,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1988,11 +2002,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="2098009"/>
-        <c:axId val="83938724"/>
+        <c:axId val="68905159"/>
+        <c:axId val="20492452"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2098009"/>
+        <c:axId val="68905159"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2058,7 +2072,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83938724"/>
+        <c:crossAx val="20492452"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2066,7 +2080,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83938724"/>
+        <c:axId val="20492452"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2142,7 +2156,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2098009"/>
+        <c:crossAx val="68905159"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2169,7 +2183,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2297,11 +2311,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="8843455"/>
-        <c:axId val="65651500"/>
+        <c:axId val="47719902"/>
+        <c:axId val="32070005"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8843455"/>
+        <c:axId val="47719902"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2367,7 +2381,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65651500"/>
+        <c:crossAx val="32070005"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2375,7 +2389,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65651500"/>
+        <c:axId val="32070005"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,7 +2465,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8843455"/>
+        <c:crossAx val="47719902"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2478,7 +2492,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2606,11 +2620,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="92736001"/>
-        <c:axId val="73664156"/>
+        <c:axId val="75774467"/>
+        <c:axId val="41413981"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92736001"/>
+        <c:axId val="75774467"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2676,7 +2690,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73664156"/>
+        <c:crossAx val="41413981"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2684,7 +2698,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73664156"/>
+        <c:axId val="41413981"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2760,7 +2774,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92736001"/>
+        <c:crossAx val="75774467"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2787,7 +2801,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2915,11 +2929,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="92640251"/>
-        <c:axId val="43462939"/>
+        <c:axId val="29450992"/>
+        <c:axId val="24224290"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92640251"/>
+        <c:axId val="29450992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2985,7 +2999,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43462939"/>
+        <c:crossAx val="24224290"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2993,7 +3007,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43462939"/>
+        <c:axId val="24224290"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3069,7 +3083,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92640251"/>
+        <c:crossAx val="29450992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3096,7 +3110,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3224,11 +3238,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="70085744"/>
-        <c:axId val="21387531"/>
+        <c:axId val="62696433"/>
+        <c:axId val="92652894"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70085744"/>
+        <c:axId val="62696433"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3294,7 +3308,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21387531"/>
+        <c:crossAx val="92652894"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3302,7 +3316,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="21387531"/>
+        <c:axId val="92652894"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3378,7 +3392,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70085744"/>
+        <c:crossAx val="62696433"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8062,8 +8076,8 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C25" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
P07 Last Item - Create Graphics 3/21/2023 7:16 AM
</commit_message>
<xml_diff>
--- a/P07/Scrum_Sprint_3.xlsx
+++ b/P07/Scrum_Sprint_3.xlsx
@@ -99,12 +99,26 @@
         </r>
       </text>
     </comment>
+    <comment ref="D35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">git commit -m "P07 Last Item - Create Graphics 3/21/2023 12:57 AM"
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="208">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -854,7 +868,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -883,12 +897,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFAEAAAA"/>
         <bgColor rgb="FFB2B2B2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF420E"/>
       </patternFill>
     </fill>
   </fills>
@@ -1144,7 +1152,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1232,7 +1240,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1384,11 +1392,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="79115450"/>
-        <c:axId val="21830319"/>
+        <c:axId val="480394"/>
+        <c:axId val="1253333"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79115450"/>
+        <c:axId val="480394"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1456,12 +1464,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21830319"/>
+        <c:crossAx val="1253333"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21830319"/>
+        <c:axId val="1253333"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1538,7 +1546,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79115450"/>
+        <c:crossAx val="480394"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1565,7 +1573,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart58.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1693,11 +1701,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="15432580"/>
-        <c:axId val="35846606"/>
+        <c:axId val="57131454"/>
+        <c:axId val="95535579"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15432580"/>
+        <c:axId val="57131454"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,7 +1771,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35846606"/>
+        <c:crossAx val="95535579"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1771,7 +1779,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35846606"/>
+        <c:axId val="95535579"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1847,7 +1855,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15432580"/>
+        <c:crossAx val="57131454"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1874,7 +1882,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart59.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2002,11 +2010,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="68905159"/>
-        <c:axId val="20492452"/>
+        <c:axId val="45399152"/>
+        <c:axId val="56621120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68905159"/>
+        <c:axId val="45399152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2072,7 +2080,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20492452"/>
+        <c:crossAx val="56621120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2080,7 +2088,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20492452"/>
+        <c:axId val="56621120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2156,7 +2164,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68905159"/>
+        <c:crossAx val="45399152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2183,7 +2191,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart60.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2275,19 +2283,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>14</c:v>
@@ -2311,11 +2319,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="47719902"/>
-        <c:axId val="32070005"/>
+        <c:axId val="71373019"/>
+        <c:axId val="45969618"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47719902"/>
+        <c:axId val="71373019"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2381,7 +2389,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32070005"/>
+        <c:crossAx val="45969618"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2389,7 +2397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32070005"/>
+        <c:axId val="45969618"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2465,7 +2473,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47719902"/>
+        <c:crossAx val="71373019"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2492,7 +2500,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart61.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2620,11 +2628,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="75774467"/>
-        <c:axId val="41413981"/>
+        <c:axId val="13209157"/>
+        <c:axId val="92538665"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75774467"/>
+        <c:axId val="13209157"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2690,7 +2698,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41413981"/>
+        <c:crossAx val="92538665"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2698,7 +2706,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41413981"/>
+        <c:axId val="92538665"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2774,7 +2782,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75774467"/>
+        <c:crossAx val="13209157"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2801,7 +2809,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart62.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2929,11 +2937,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="29450992"/>
-        <c:axId val="24224290"/>
+        <c:axId val="52442538"/>
+        <c:axId val="11571746"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="29450992"/>
+        <c:axId val="52442538"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2999,7 +3007,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24224290"/>
+        <c:crossAx val="11571746"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3007,7 +3015,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="24224290"/>
+        <c:axId val="11571746"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3083,7 +3091,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29450992"/>
+        <c:crossAx val="52442538"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3110,7 +3118,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart63.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3238,11 +3246,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="62696433"/>
-        <c:axId val="92652894"/>
+        <c:axId val="24432787"/>
+        <c:axId val="20025306"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62696433"/>
+        <c:axId val="24432787"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3308,7 +3316,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92652894"/>
+        <c:crossAx val="20025306"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3316,7 +3324,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92652894"/>
+        <c:axId val="20025306"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3392,7 +3400,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62696433"/>
+        <c:crossAx val="24432787"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3673,7 +3681,7 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+      <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8076,8 +8084,8 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C25" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8169,7 +8177,7 @@
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -8182,7 +8190,7 @@
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">B7-C8</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -8198,7 +8206,7 @@
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">B8-C9</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -8214,7 +8222,7 @@
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">B9-C10</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -8230,7 +8238,7 @@
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">B10-C11</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -8250,7 +8258,7 @@
       </c>
       <c r="C12" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
@@ -8562,7 +8570,7 @@
         <v>202</v>
       </c>
       <c r="E31" s="44" t="s">
-        <v>81</v>
+        <v>168</v>
       </c>
       <c r="F31" s="45"/>
     </row>
@@ -8620,14 +8628,20 @@
         <v>161</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B35" s="42"/>
+      <c r="B35" s="42" t="s">
+        <v>80</v>
+      </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="44"/>
+      <c r="D35" s="48" t="s">
+        <v>205</v>
+      </c>
+      <c r="E35" s="44" t="s">
+        <v>81</v>
+      </c>
       <c r="F35" s="45"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>